<commit_message>
test of class Quartier
</commit_message>
<xml_diff>
--- a/src/ressources/cahierDeTests.xlsx
+++ b/src/ressources/cahierDeTests.xlsx
@@ -1,16 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24527"/>
-  <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\palbers\Documents\Cours\ProjetDeveloppementJavaIR3\Document\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{67BD7D02-CAC0-44EE-9A22-B0A312B4F6CB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="11430" windowHeight="3765" firstSheet="1" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Objectifs" sheetId="1" r:id="rId1"/>
@@ -21,7 +15,8 @@
     <sheet name="test.TestPlateauDeJeu" sheetId="6" r:id="rId6"/>
     <sheet name="test..." sheetId="7" r:id="rId7"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="0"/>
+  <oleSize ref="E2:J7"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -40,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="40">
   <si>
     <t>Objectif</t>
   </si>
@@ -164,12 +159,18 @@
   </si>
   <si>
     <t>TestJoueur.test5()</t>
+  </si>
+  <si>
+    <t>Gilles Cédric</t>
+  </si>
+  <si>
+    <t>OK</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -416,7 +417,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -444,6 +445,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -757,34 +759,34 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:B5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="77.21875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="77.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:2" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="2" spans="2:2" ht="45" x14ac:dyDescent="0.25">
       <c r="B2" s="1" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="3" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="4" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="5" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
         <v>31</v>
       </c>
@@ -795,28 +797,30 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:K26"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="B2" workbookViewId="0">
+      <selection activeCell="D5" sqref="D5"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="3.5546875" customWidth="1"/>
-    <col min="2" max="2" width="20.77734375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="18.109375" customWidth="1"/>
-    <col min="4" max="4" width="27.77734375" customWidth="1"/>
-    <col min="5" max="5" width="12.77734375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="8.88671875" customWidth="1"/>
+    <col min="1" max="1" width="3.5703125" customWidth="1"/>
+    <col min="2" max="2" width="20.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.140625" customWidth="1"/>
+    <col min="4" max="4" width="27.7109375" customWidth="1"/>
+    <col min="5" max="5" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="8.85546875" customWidth="1"/>
     <col min="7" max="7" width="31" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="8.109375" customWidth="1"/>
-    <col min="9" max="9" width="9.109375" customWidth="1"/>
-    <col min="10" max="10" width="21.44140625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="48.109375" customWidth="1"/>
+    <col min="8" max="8" width="11.7109375" customWidth="1"/>
+    <col min="9" max="9" width="9.140625" customWidth="1"/>
+    <col min="10" max="10" width="21.42578125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="48.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:11" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="2" spans="2:11" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="2" spans="2:11" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B2" s="11" t="s">
         <v>13</v>
       </c>
@@ -848,7 +852,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B3" s="8" t="s">
         <v>9</v>
       </c>
@@ -867,12 +871,18 @@
       <c r="G3" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="H3" s="9"/>
-      <c r="I3" s="9"/>
-      <c r="J3" s="9"/>
+      <c r="H3" s="19">
+        <v>44515</v>
+      </c>
+      <c r="I3" s="9" t="s">
+        <v>38</v>
+      </c>
+      <c r="J3" s="9" t="s">
+        <v>39</v>
+      </c>
       <c r="K3" s="10"/>
     </row>
-    <row r="4" spans="2:11" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:11" ht="30" x14ac:dyDescent="0.25">
       <c r="B4" s="8" t="s">
         <v>9</v>
       </c>
@@ -896,7 +906,7 @@
       <c r="J4" s="2"/>
       <c r="K4" s="4"/>
     </row>
-    <row r="5" spans="2:11" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:11" ht="30" x14ac:dyDescent="0.25">
       <c r="B5" s="8" t="s">
         <v>9</v>
       </c>
@@ -920,7 +930,7 @@
       <c r="J5" s="2"/>
       <c r="K5" s="4"/>
     </row>
-    <row r="6" spans="2:11" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:11" ht="30" x14ac:dyDescent="0.25">
       <c r="B6" s="8" t="s">
         <v>9</v>
       </c>
@@ -944,7 +954,7 @@
       <c r="J6" s="2"/>
       <c r="K6" s="4"/>
     </row>
-    <row r="7" spans="2:11" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:11" ht="30" x14ac:dyDescent="0.25">
       <c r="B7" s="8" t="s">
         <v>9</v>
       </c>
@@ -968,7 +978,7 @@
       <c r="J7" s="2"/>
       <c r="K7" s="4"/>
     </row>
-    <row r="8" spans="2:11" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="8" spans="2:11" ht="30" x14ac:dyDescent="0.25">
       <c r="B8" s="8" t="s">
         <v>9</v>
       </c>
@@ -992,7 +1002,7 @@
       <c r="J8" s="2"/>
       <c r="K8" s="4"/>
     </row>
-    <row r="9" spans="2:11" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="9" spans="2:11" ht="30" x14ac:dyDescent="0.25">
       <c r="B9" s="8" t="s">
         <v>9</v>
       </c>
@@ -1016,7 +1026,7 @@
       <c r="J9" s="2"/>
       <c r="K9" s="4"/>
     </row>
-    <row r="10" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="10" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B10" s="3"/>
       <c r="C10" s="16"/>
       <c r="D10" s="2"/>
@@ -1028,7 +1038,7 @@
       <c r="J10" s="2"/>
       <c r="K10" s="4"/>
     </row>
-    <row r="11" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="11" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B11" s="3"/>
       <c r="C11" s="16"/>
       <c r="D11" s="2"/>
@@ -1040,7 +1050,7 @@
       <c r="J11" s="2"/>
       <c r="K11" s="4"/>
     </row>
-    <row r="12" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="12" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B12" s="3"/>
       <c r="C12" s="16"/>
       <c r="D12" s="2"/>
@@ -1052,7 +1062,7 @@
       <c r="J12" s="2"/>
       <c r="K12" s="4"/>
     </row>
-    <row r="13" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="13" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B13" s="3"/>
       <c r="C13" s="16"/>
       <c r="D13" s="2"/>
@@ -1064,7 +1074,7 @@
       <c r="J13" s="2"/>
       <c r="K13" s="4"/>
     </row>
-    <row r="14" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="14" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B14" s="3"/>
       <c r="C14" s="16"/>
       <c r="D14" s="2"/>
@@ -1076,7 +1086,7 @@
       <c r="J14" s="2"/>
       <c r="K14" s="4"/>
     </row>
-    <row r="15" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="15" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B15" s="3"/>
       <c r="C15" s="16"/>
       <c r="D15" s="2"/>
@@ -1088,7 +1098,7 @@
       <c r="J15" s="2"/>
       <c r="K15" s="4"/>
     </row>
-    <row r="16" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="16" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B16" s="3"/>
       <c r="C16" s="16"/>
       <c r="D16" s="2"/>
@@ -1100,7 +1110,7 @@
       <c r="J16" s="2"/>
       <c r="K16" s="4"/>
     </row>
-    <row r="17" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B17" s="3"/>
       <c r="C17" s="16"/>
       <c r="D17" s="2"/>
@@ -1112,7 +1122,7 @@
       <c r="J17" s="2"/>
       <c r="K17" s="4"/>
     </row>
-    <row r="18" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="18" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B18" s="3"/>
       <c r="C18" s="16"/>
       <c r="D18" s="2"/>
@@ -1124,7 +1134,7 @@
       <c r="J18" s="2"/>
       <c r="K18" s="4"/>
     </row>
-    <row r="19" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="19" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B19" s="3"/>
       <c r="C19" s="16"/>
       <c r="D19" s="2"/>
@@ -1136,7 +1146,7 @@
       <c r="J19" s="2"/>
       <c r="K19" s="4"/>
     </row>
-    <row r="20" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="20" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B20" s="3"/>
       <c r="C20" s="16"/>
       <c r="D20" s="2"/>
@@ -1148,7 +1158,7 @@
       <c r="J20" s="2"/>
       <c r="K20" s="4"/>
     </row>
-    <row r="21" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="21" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B21" s="3"/>
       <c r="C21" s="16"/>
       <c r="D21" s="2"/>
@@ -1160,7 +1170,7 @@
       <c r="J21" s="2"/>
       <c r="K21" s="4"/>
     </row>
-    <row r="22" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="22" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B22" s="3"/>
       <c r="C22" s="16"/>
       <c r="D22" s="2"/>
@@ -1172,7 +1182,7 @@
       <c r="J22" s="2"/>
       <c r="K22" s="4"/>
     </row>
-    <row r="23" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="23" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B23" s="3"/>
       <c r="C23" s="16"/>
       <c r="D23" s="2"/>
@@ -1184,7 +1194,7 @@
       <c r="J23" s="2"/>
       <c r="K23" s="4"/>
     </row>
-    <row r="24" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="24" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B24" s="3"/>
       <c r="C24" s="16"/>
       <c r="D24" s="2"/>
@@ -1196,7 +1206,7 @@
       <c r="J24" s="2"/>
       <c r="K24" s="4"/>
     </row>
-    <row r="25" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="25" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B25" s="3"/>
       <c r="C25" s="16"/>
       <c r="D25" s="2"/>
@@ -1208,7 +1218,7 @@
       <c r="J25" s="2"/>
       <c r="K25" s="4"/>
     </row>
-    <row r="26" spans="2:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="26" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B26" s="5"/>
       <c r="C26" s="17"/>
       <c r="D26" s="6"/>
@@ -1226,29 +1236,29 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E5701002-B3A8-41DB-8C9E-5154A0ED617D}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:K26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection sqref="A1:L26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="21.5546875" customWidth="1"/>
-    <col min="3" max="3" width="19.77734375" customWidth="1"/>
-    <col min="4" max="4" width="23.88671875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.5546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="7.44140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="21.5703125" customWidth="1"/>
+    <col min="3" max="3" width="19.7109375" customWidth="1"/>
+    <col min="4" max="4" width="23.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="7.42578125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="31" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="5" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="7.44140625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="27.88671875" customWidth="1"/>
-    <col min="11" max="11" width="59.33203125" customWidth="1"/>
+    <col min="9" max="9" width="7.42578125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="27.85546875" customWidth="1"/>
+    <col min="11" max="11" width="59.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:11" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="2" spans="2:11" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="2" spans="2:11" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B2" s="11" t="s">
         <v>13</v>
       </c>
@@ -1280,7 +1290,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B3" s="8" t="s">
         <v>9</v>
       </c>
@@ -1296,7 +1306,7 @@
       <c r="J3" s="9"/>
       <c r="K3" s="10"/>
     </row>
-    <row r="4" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B4" s="8" t="s">
         <v>9</v>
       </c>
@@ -1312,7 +1322,7 @@
       <c r="J4" s="2"/>
       <c r="K4" s="4"/>
     </row>
-    <row r="5" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B5" s="8" t="s">
         <v>9</v>
       </c>
@@ -1328,7 +1338,7 @@
       <c r="J5" s="2"/>
       <c r="K5" s="4"/>
     </row>
-    <row r="6" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B6" s="8" t="s">
         <v>9</v>
       </c>
@@ -1344,7 +1354,7 @@
       <c r="J6" s="2"/>
       <c r="K6" s="4"/>
     </row>
-    <row r="7" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B7" s="8" t="s">
         <v>9</v>
       </c>
@@ -1360,7 +1370,7 @@
       <c r="J7" s="2"/>
       <c r="K7" s="4"/>
     </row>
-    <row r="8" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="8" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B8" s="8"/>
       <c r="C8" s="15"/>
       <c r="D8" s="18"/>
@@ -1372,7 +1382,7 @@
       <c r="J8" s="2"/>
       <c r="K8" s="4"/>
     </row>
-    <row r="9" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="9" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B9" s="8"/>
       <c r="C9" s="15"/>
       <c r="D9" s="18"/>
@@ -1384,7 +1394,7 @@
       <c r="J9" s="2"/>
       <c r="K9" s="4"/>
     </row>
-    <row r="10" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="10" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B10" s="3"/>
       <c r="C10" s="16"/>
       <c r="D10" s="2"/>
@@ -1396,7 +1406,7 @@
       <c r="J10" s="2"/>
       <c r="K10" s="4"/>
     </row>
-    <row r="11" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="11" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B11" s="3"/>
       <c r="C11" s="16"/>
       <c r="D11" s="2"/>
@@ -1408,7 +1418,7 @@
       <c r="J11" s="2"/>
       <c r="K11" s="4"/>
     </row>
-    <row r="12" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="12" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B12" s="3"/>
       <c r="C12" s="16"/>
       <c r="D12" s="2"/>
@@ -1420,7 +1430,7 @@
       <c r="J12" s="2"/>
       <c r="K12" s="4"/>
     </row>
-    <row r="13" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="13" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B13" s="3"/>
       <c r="C13" s="16"/>
       <c r="D13" s="2"/>
@@ -1432,7 +1442,7 @@
       <c r="J13" s="2"/>
       <c r="K13" s="4"/>
     </row>
-    <row r="14" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="14" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B14" s="3"/>
       <c r="C14" s="16"/>
       <c r="D14" s="2"/>
@@ -1444,7 +1454,7 @@
       <c r="J14" s="2"/>
       <c r="K14" s="4"/>
     </row>
-    <row r="15" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="15" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B15" s="3"/>
       <c r="C15" s="16"/>
       <c r="D15" s="2"/>
@@ -1456,7 +1466,7 @@
       <c r="J15" s="2"/>
       <c r="K15" s="4"/>
     </row>
-    <row r="16" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="16" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B16" s="3"/>
       <c r="C16" s="16"/>
       <c r="D16" s="2"/>
@@ -1468,7 +1478,7 @@
       <c r="J16" s="2"/>
       <c r="K16" s="4"/>
     </row>
-    <row r="17" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B17" s="3"/>
       <c r="C17" s="16"/>
       <c r="D17" s="2"/>
@@ -1480,7 +1490,7 @@
       <c r="J17" s="2"/>
       <c r="K17" s="4"/>
     </row>
-    <row r="18" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="18" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B18" s="3"/>
       <c r="C18" s="16"/>
       <c r="D18" s="2"/>
@@ -1492,7 +1502,7 @@
       <c r="J18" s="2"/>
       <c r="K18" s="4"/>
     </row>
-    <row r="19" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="19" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B19" s="3"/>
       <c r="C19" s="16"/>
       <c r="D19" s="2"/>
@@ -1504,7 +1514,7 @@
       <c r="J19" s="2"/>
       <c r="K19" s="4"/>
     </row>
-    <row r="20" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="20" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B20" s="3"/>
       <c r="C20" s="16"/>
       <c r="D20" s="2"/>
@@ -1516,7 +1526,7 @@
       <c r="J20" s="2"/>
       <c r="K20" s="4"/>
     </row>
-    <row r="21" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="21" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B21" s="3"/>
       <c r="C21" s="16"/>
       <c r="D21" s="2"/>
@@ -1528,7 +1538,7 @@
       <c r="J21" s="2"/>
       <c r="K21" s="4"/>
     </row>
-    <row r="22" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="22" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B22" s="3"/>
       <c r="C22" s="16"/>
       <c r="D22" s="2"/>
@@ -1540,7 +1550,7 @@
       <c r="J22" s="2"/>
       <c r="K22" s="4"/>
     </row>
-    <row r="23" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="23" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B23" s="3"/>
       <c r="C23" s="16"/>
       <c r="D23" s="2"/>
@@ -1552,7 +1562,7 @@
       <c r="J23" s="2"/>
       <c r="K23" s="4"/>
     </row>
-    <row r="24" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="24" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B24" s="3"/>
       <c r="C24" s="16"/>
       <c r="D24" s="2"/>
@@ -1564,7 +1574,7 @@
       <c r="J24" s="2"/>
       <c r="K24" s="4"/>
     </row>
-    <row r="25" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="25" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B25" s="3"/>
       <c r="C25" s="16"/>
       <c r="D25" s="2"/>
@@ -1576,7 +1586,7 @@
       <c r="J25" s="2"/>
       <c r="K25" s="4"/>
     </row>
-    <row r="26" spans="2:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="26" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B26" s="5"/>
       <c r="C26" s="17"/>
       <c r="D26" s="6"/>
@@ -1594,28 +1604,28 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1ACBC47F-1DC7-4885-9E4E-0C9BB500AA8A}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:K26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="N7" sqref="N7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="21.109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="19.33203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="7.88671875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.5546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="7.44140625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="17.109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="21.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="7.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="7.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="17.140625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="5" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="7.44140625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="22.77734375" customWidth="1"/>
+    <col min="9" max="9" width="7.42578125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="22.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:11" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="2" spans="2:11" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="2" spans="2:11" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B2" s="11" t="s">
         <v>13</v>
       </c>
@@ -1647,7 +1657,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B3" s="8"/>
       <c r="C3" s="15"/>
       <c r="D3" s="9"/>
@@ -1659,7 +1669,7 @@
       <c r="J3" s="9"/>
       <c r="K3" s="10"/>
     </row>
-    <row r="4" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B4" s="8"/>
       <c r="C4" s="15"/>
       <c r="D4" s="18"/>
@@ -1671,7 +1681,7 @@
       <c r="J4" s="2"/>
       <c r="K4" s="4"/>
     </row>
-    <row r="5" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B5" s="8"/>
       <c r="C5" s="15"/>
       <c r="D5" s="18"/>
@@ -1683,7 +1693,7 @@
       <c r="J5" s="2"/>
       <c r="K5" s="4"/>
     </row>
-    <row r="6" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B6" s="8"/>
       <c r="C6" s="15"/>
       <c r="D6" s="18"/>
@@ -1695,7 +1705,7 @@
       <c r="J6" s="2"/>
       <c r="K6" s="4"/>
     </row>
-    <row r="7" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B7" s="8"/>
       <c r="C7" s="15"/>
       <c r="D7" s="18"/>
@@ -1707,7 +1717,7 @@
       <c r="J7" s="2"/>
       <c r="K7" s="4"/>
     </row>
-    <row r="8" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="8" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B8" s="8"/>
       <c r="C8" s="15"/>
       <c r="D8" s="18"/>
@@ -1719,7 +1729,7 @@
       <c r="J8" s="2"/>
       <c r="K8" s="4"/>
     </row>
-    <row r="9" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="9" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B9" s="8"/>
       <c r="C9" s="15"/>
       <c r="D9" s="18"/>
@@ -1731,7 +1741,7 @@
       <c r="J9" s="2"/>
       <c r="K9" s="4"/>
     </row>
-    <row r="10" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="10" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B10" s="3"/>
       <c r="C10" s="16"/>
       <c r="D10" s="2"/>
@@ -1743,7 +1753,7 @@
       <c r="J10" s="2"/>
       <c r="K10" s="4"/>
     </row>
-    <row r="11" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="11" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B11" s="3"/>
       <c r="C11" s="16"/>
       <c r="D11" s="2"/>
@@ -1755,7 +1765,7 @@
       <c r="J11" s="2"/>
       <c r="K11" s="4"/>
     </row>
-    <row r="12" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="12" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B12" s="3"/>
       <c r="C12" s="16"/>
       <c r="D12" s="2"/>
@@ -1767,7 +1777,7 @@
       <c r="J12" s="2"/>
       <c r="K12" s="4"/>
     </row>
-    <row r="13" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="13" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B13" s="3"/>
       <c r="C13" s="16"/>
       <c r="D13" s="2"/>
@@ -1779,7 +1789,7 @@
       <c r="J13" s="2"/>
       <c r="K13" s="4"/>
     </row>
-    <row r="14" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="14" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B14" s="3"/>
       <c r="C14" s="16"/>
       <c r="D14" s="2"/>
@@ -1791,7 +1801,7 @@
       <c r="J14" s="2"/>
       <c r="K14" s="4"/>
     </row>
-    <row r="15" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="15" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B15" s="3"/>
       <c r="C15" s="16"/>
       <c r="D15" s="2"/>
@@ -1803,7 +1813,7 @@
       <c r="J15" s="2"/>
       <c r="K15" s="4"/>
     </row>
-    <row r="16" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="16" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B16" s="3"/>
       <c r="C16" s="16"/>
       <c r="D16" s="2"/>
@@ -1815,7 +1825,7 @@
       <c r="J16" s="2"/>
       <c r="K16" s="4"/>
     </row>
-    <row r="17" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B17" s="3"/>
       <c r="C17" s="16"/>
       <c r="D17" s="2"/>
@@ -1827,7 +1837,7 @@
       <c r="J17" s="2"/>
       <c r="K17" s="4"/>
     </row>
-    <row r="18" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="18" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B18" s="3"/>
       <c r="C18" s="16"/>
       <c r="D18" s="2"/>
@@ -1839,7 +1849,7 @@
       <c r="J18" s="2"/>
       <c r="K18" s="4"/>
     </row>
-    <row r="19" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="19" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B19" s="3"/>
       <c r="C19" s="16"/>
       <c r="D19" s="2"/>
@@ -1851,7 +1861,7 @@
       <c r="J19" s="2"/>
       <c r="K19" s="4"/>
     </row>
-    <row r="20" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="20" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B20" s="3"/>
       <c r="C20" s="16"/>
       <c r="D20" s="2"/>
@@ -1863,7 +1873,7 @@
       <c r="J20" s="2"/>
       <c r="K20" s="4"/>
     </row>
-    <row r="21" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="21" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B21" s="3"/>
       <c r="C21" s="16"/>
       <c r="D21" s="2"/>
@@ -1875,7 +1885,7 @@
       <c r="J21" s="2"/>
       <c r="K21" s="4"/>
     </row>
-    <row r="22" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="22" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B22" s="3"/>
       <c r="C22" s="16"/>
       <c r="D22" s="2"/>
@@ -1887,7 +1897,7 @@
       <c r="J22" s="2"/>
       <c r="K22" s="4"/>
     </row>
-    <row r="23" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="23" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B23" s="3"/>
       <c r="C23" s="16"/>
       <c r="D23" s="2"/>
@@ -1899,7 +1909,7 @@
       <c r="J23" s="2"/>
       <c r="K23" s="4"/>
     </row>
-    <row r="24" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="24" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B24" s="3"/>
       <c r="C24" s="16"/>
       <c r="D24" s="2"/>
@@ -1911,7 +1921,7 @@
       <c r="J24" s="2"/>
       <c r="K24" s="4"/>
     </row>
-    <row r="25" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="25" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B25" s="3"/>
       <c r="C25" s="16"/>
       <c r="D25" s="2"/>
@@ -1923,7 +1933,7 @@
       <c r="J25" s="2"/>
       <c r="K25" s="4"/>
     </row>
-    <row r="26" spans="2:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="26" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B26" s="5"/>
       <c r="C26" s="17"/>
       <c r="D26" s="6"/>
@@ -1941,38 +1951,38 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2A3A52A6-55C3-43DC-9913-0090E55DBF07}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="H30" sqref="H30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{526A09AA-D1AE-4FBD-9776-3D5002FF76D5}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{48E35FE0-6337-4AA7-8A06-879FAEE5A39F}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
test of class Roi and correction of bugs in class Roi and class Joueur
</commit_message>
<xml_diff>
--- a/src/ressources/cahierDeTests.xlsx
+++ b/src/ressources/cahierDeTests.xlsx
@@ -3,8 +3,13 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\HP\eclipse-2021-workspace\Citadelle\src\ressources\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="11430" windowHeight="3765" firstSheet="1" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="11430" windowHeight="3765" firstSheet="1" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Objectifs" sheetId="1" r:id="rId1"/>
@@ -16,7 +21,6 @@
     <sheet name="test..." sheetId="7" r:id="rId7"/>
   </sheets>
   <calcPr calcId="0"/>
-  <oleSize ref="E2:J7"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -35,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="156" uniqueCount="48">
   <si>
     <t>Objectif</t>
   </si>
@@ -165,6 +169,31 @@
   </si>
   <si>
     <t>OK</t>
+  </si>
+  <si>
+    <t>tester le constructeur</t>
+  </si>
+  <si>
+    <t>tous les champs sont bien affectés ou nuls</t>
+  </si>
+  <si>
+    <t>TEST DE L'ATTRIBUTION D'UN JOUEUR
+ un quartier religieux</t>
+  </si>
+  <si>
+    <t>le nom du joueur doit être changé</t>
+  </si>
+  <si>
+    <t>TEST DE L'ASSASSINAT DU PERSONNAGE</t>
+  </si>
+  <si>
+    <t>le champ assassine doit etre changé en true</t>
+  </si>
+  <si>
+    <t>TEST DU VOL DU PERSONNAGE</t>
+  </si>
+  <si>
+    <t>le champ vole doit etre changé en true</t>
   </si>
 </sst>
 </file>
@@ -800,8 +829,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:K26"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B2" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+    <sheetView topLeftCell="B2" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3:J9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -901,9 +930,15 @@
       <c r="G4" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="H4" s="2"/>
-      <c r="I4" s="2"/>
-      <c r="J4" s="2"/>
+      <c r="H4" s="19">
+        <v>44515</v>
+      </c>
+      <c r="I4" s="9" t="s">
+        <v>38</v>
+      </c>
+      <c r="J4" s="9" t="s">
+        <v>39</v>
+      </c>
       <c r="K4" s="4"/>
     </row>
     <row r="5" spans="2:11" ht="30" x14ac:dyDescent="0.25">
@@ -925,9 +960,15 @@
       <c r="G5" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="H5" s="2"/>
-      <c r="I5" s="2"/>
-      <c r="J5" s="2"/>
+      <c r="H5" s="19">
+        <v>44515</v>
+      </c>
+      <c r="I5" s="9" t="s">
+        <v>38</v>
+      </c>
+      <c r="J5" s="9" t="s">
+        <v>39</v>
+      </c>
       <c r="K5" s="4"/>
     </row>
     <row r="6" spans="2:11" ht="30" x14ac:dyDescent="0.25">
@@ -949,9 +990,15 @@
       <c r="G6" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="H6" s="2"/>
-      <c r="I6" s="2"/>
-      <c r="J6" s="2"/>
+      <c r="H6" s="19">
+        <v>44515</v>
+      </c>
+      <c r="I6" s="9" t="s">
+        <v>38</v>
+      </c>
+      <c r="J6" s="9" t="s">
+        <v>39</v>
+      </c>
       <c r="K6" s="4"/>
     </row>
     <row r="7" spans="2:11" ht="30" x14ac:dyDescent="0.25">
@@ -973,9 +1020,15 @@
       <c r="G7" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="H7" s="2"/>
-      <c r="I7" s="2"/>
-      <c r="J7" s="2"/>
+      <c r="H7" s="19">
+        <v>44515</v>
+      </c>
+      <c r="I7" s="9" t="s">
+        <v>38</v>
+      </c>
+      <c r="J7" s="9" t="s">
+        <v>39</v>
+      </c>
       <c r="K7" s="4"/>
     </row>
     <row r="8" spans="2:11" ht="30" x14ac:dyDescent="0.25">
@@ -997,9 +1050,15 @@
       <c r="G8" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="H8" s="2"/>
-      <c r="I8" s="2"/>
-      <c r="J8" s="2"/>
+      <c r="H8" s="19">
+        <v>44515</v>
+      </c>
+      <c r="I8" s="9" t="s">
+        <v>38</v>
+      </c>
+      <c r="J8" s="9" t="s">
+        <v>39</v>
+      </c>
       <c r="K8" s="4"/>
     </row>
     <row r="9" spans="2:11" ht="30" x14ac:dyDescent="0.25">
@@ -1021,9 +1080,15 @@
       <c r="G9" s="18" t="s">
         <v>28</v>
       </c>
-      <c r="H9" s="2"/>
-      <c r="I9" s="2"/>
-      <c r="J9" s="2"/>
+      <c r="H9" s="19">
+        <v>44515</v>
+      </c>
+      <c r="I9" s="9" t="s">
+        <v>38</v>
+      </c>
+      <c r="J9" s="9" t="s">
+        <v>39</v>
+      </c>
       <c r="K9" s="4"/>
     </row>
     <row r="10" spans="2:11" x14ac:dyDescent="0.25">
@@ -1240,7 +1305,7 @@
   <dimension ref="B1:K26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:L26"/>
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1607,20 +1672,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:K26"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="N7" sqref="N7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="21.140625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="19.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="7.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="31.7109375" customWidth="1"/>
     <col min="5" max="5" width="13.5703125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="7.42578125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="17.140625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="5" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="7.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="31.28515625" customWidth="1"/>
+    <col min="8" max="8" width="12.7109375" customWidth="1"/>
+    <col min="9" max="9" width="13.5703125" customWidth="1"/>
     <col min="10" max="10" width="22.7109375" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1658,87 +1723,213 @@
       </c>
     </row>
     <row r="3" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B3" s="8"/>
-      <c r="C3" s="15"/>
-      <c r="D3" s="9"/>
-      <c r="E3" s="9"/>
-      <c r="F3" s="9"/>
-      <c r="G3" s="9"/>
-      <c r="H3" s="9"/>
-      <c r="I3" s="9"/>
-      <c r="J3" s="9"/>
+      <c r="B3" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="C3" s="15" t="s">
+        <v>14</v>
+      </c>
+      <c r="D3" s="9" t="s">
+        <v>40</v>
+      </c>
+      <c r="E3" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="F3" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="G3" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="H3" s="19">
+        <v>44515</v>
+      </c>
+      <c r="I3" s="9" t="s">
+        <v>38</v>
+      </c>
+      <c r="J3" s="9" t="s">
+        <v>39</v>
+      </c>
       <c r="K3" s="10"/>
     </row>
-    <row r="4" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B4" s="8"/>
-      <c r="C4" s="15"/>
-      <c r="D4" s="18"/>
-      <c r="E4" s="9"/>
-      <c r="F4" s="9"/>
-      <c r="G4" s="9"/>
-      <c r="H4" s="2"/>
-      <c r="I4" s="2"/>
-      <c r="J4" s="2"/>
+    <row r="4" spans="2:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B4" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="C4" s="15" t="s">
+        <v>15</v>
+      </c>
+      <c r="D4" s="18" t="s">
+        <v>42</v>
+      </c>
+      <c r="E4" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="F4" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="G4" s="9" t="s">
+        <v>43</v>
+      </c>
+      <c r="H4" s="19">
+        <v>44515</v>
+      </c>
+      <c r="I4" s="9" t="s">
+        <v>38</v>
+      </c>
+      <c r="J4" s="9" t="s">
+        <v>39</v>
+      </c>
       <c r="K4" s="4"/>
     </row>
-    <row r="5" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B5" s="8"/>
-      <c r="C5" s="15"/>
-      <c r="D5" s="18"/>
-      <c r="E5" s="9"/>
-      <c r="F5" s="9"/>
-      <c r="G5" s="9"/>
-      <c r="H5" s="2"/>
-      <c r="I5" s="2"/>
-      <c r="J5" s="2"/>
+    <row r="5" spans="2:11" ht="30" x14ac:dyDescent="0.25">
+      <c r="B5" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="C5" s="15" t="s">
+        <v>18</v>
+      </c>
+      <c r="D5" s="18" t="s">
+        <v>44</v>
+      </c>
+      <c r="E5" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="F5" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="G5" s="9" t="s">
+        <v>45</v>
+      </c>
+      <c r="H5" s="19">
+        <v>44515</v>
+      </c>
+      <c r="I5" s="9" t="s">
+        <v>38</v>
+      </c>
+      <c r="J5" s="9" t="s">
+        <v>39</v>
+      </c>
       <c r="K5" s="4"/>
     </row>
-    <row r="6" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B6" s="8"/>
-      <c r="C6" s="15"/>
-      <c r="D6" s="18"/>
-      <c r="E6" s="9"/>
-      <c r="F6" s="9"/>
-      <c r="G6" s="9"/>
-      <c r="H6" s="2"/>
-      <c r="I6" s="2"/>
-      <c r="J6" s="2"/>
+    <row r="6" spans="2:11" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B6" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="C6" s="15" t="s">
+        <v>21</v>
+      </c>
+      <c r="D6" s="18" t="s">
+        <v>46</v>
+      </c>
+      <c r="E6" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="F6" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="G6" s="9" t="s">
+        <v>47</v>
+      </c>
+      <c r="H6" s="19">
+        <v>44515</v>
+      </c>
+      <c r="I6" s="9" t="s">
+        <v>38</v>
+      </c>
+      <c r="J6" s="9" t="s">
+        <v>39</v>
+      </c>
       <c r="K6" s="4"/>
     </row>
-    <row r="7" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B7" s="8"/>
-      <c r="C7" s="15"/>
-      <c r="D7" s="18"/>
-      <c r="E7" s="9"/>
-      <c r="F7" s="9"/>
-      <c r="G7" s="9"/>
-      <c r="H7" s="2"/>
-      <c r="I7" s="2"/>
-      <c r="J7" s="2"/>
+    <row r="7" spans="2:11" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B7" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="C7" s="15" t="s">
+        <v>22</v>
+      </c>
+      <c r="D7" s="18" t="s">
+        <v>23</v>
+      </c>
+      <c r="E7" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="F7" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="G7" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="H7" s="19">
+        <v>44515</v>
+      </c>
+      <c r="I7" s="9" t="s">
+        <v>38</v>
+      </c>
+      <c r="J7" s="9" t="s">
+        <v>39</v>
+      </c>
       <c r="K7" s="4"/>
     </row>
-    <row r="8" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B8" s="8"/>
-      <c r="C8" s="15"/>
-      <c r="D8" s="18"/>
-      <c r="E8" s="9"/>
-      <c r="F8" s="9"/>
-      <c r="G8" s="9"/>
-      <c r="H8" s="2"/>
-      <c r="I8" s="2"/>
-      <c r="J8" s="2"/>
+    <row r="8" spans="2:11" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B8" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="C8" s="15" t="s">
+        <v>24</v>
+      </c>
+      <c r="D8" s="18" t="s">
+        <v>25</v>
+      </c>
+      <c r="E8" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="F8" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="G8" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="H8" s="19">
+        <v>44515</v>
+      </c>
+      <c r="I8" s="9" t="s">
+        <v>38</v>
+      </c>
+      <c r="J8" s="9" t="s">
+        <v>39</v>
+      </c>
       <c r="K8" s="4"/>
     </row>
-    <row r="9" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B9" s="8"/>
-      <c r="C9" s="15"/>
-      <c r="D9" s="18"/>
-      <c r="E9" s="9"/>
-      <c r="F9" s="9"/>
-      <c r="G9" s="18"/>
-      <c r="H9" s="2"/>
-      <c r="I9" s="2"/>
-      <c r="J9" s="2"/>
+    <row r="9" spans="2:11" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B9" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="C9" s="15" t="s">
+        <v>26</v>
+      </c>
+      <c r="D9" s="18" t="s">
+        <v>27</v>
+      </c>
+      <c r="E9" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="F9" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="G9" s="18" t="s">
+        <v>28</v>
+      </c>
+      <c r="H9" s="19">
+        <v>44515</v>
+      </c>
+      <c r="I9" s="9" t="s">
+        <v>38</v>
+      </c>
+      <c r="J9" s="9" t="s">
+        <v>39</v>
+      </c>
       <c r="K9" s="4"/>
     </row>
     <row r="10" spans="2:11" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
implémentation de la classe Interaction et de la classe Magicienne Modification de la classe Joueur et Personnage Test de la classe MAGICIENNE
</commit_message>
<xml_diff>
--- a/src/ressources/cahierDeTests.xlsx
+++ b/src/ressources/cahierDeTests.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="11430" windowHeight="3765" firstSheet="1" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="11430" windowHeight="3765" firstSheet="3" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="Objectifs" sheetId="1" r:id="rId1"/>
@@ -19,6 +19,7 @@
     <sheet name="test.TestPioche" sheetId="5" r:id="rId5"/>
     <sheet name="test.TestPlateauDeJeu" sheetId="6" r:id="rId6"/>
     <sheet name="test..." sheetId="7" r:id="rId7"/>
+    <sheet name="test.TestMagicienne" sheetId="8" r:id="rId8"/>
   </sheets>
   <calcPr calcId="0"/>
   <extLst>
@@ -39,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="156" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="356" uniqueCount="79">
   <si>
     <t>Objectif</t>
   </si>
@@ -177,13 +178,6 @@
     <t>tous les champs sont bien affectés ou nuls</t>
   </si>
   <si>
-    <t>TEST DE L'ATTRIBUTION D'UN JOUEUR
- un quartier religieux</t>
-  </si>
-  <si>
-    <t>le nom du joueur doit être changé</t>
-  </si>
-  <si>
     <t>TEST DE L'ASSASSINAT DU PERSONNAGE</t>
   </si>
   <si>
@@ -194,6 +188,105 @@
   </si>
   <si>
     <t>le champ vole doit etre changé en true</t>
+  </si>
+  <si>
+    <t>TEST DU TRESOR DU JOUEUR</t>
+  </si>
+  <si>
+    <t>le trésor doit avoir la bonne valeur</t>
+  </si>
+  <si>
+    <t>TEST DE LA CITE DU JOUEUR</t>
+  </si>
+  <si>
+    <t>la cité du joueur a bien été modifiée et possède les bons quartiers</t>
+  </si>
+  <si>
+    <t>TEST DE LA MAIN DU JOUEUR</t>
+  </si>
+  <si>
+    <t>la main du joueur a bien été modifiée et possède les bons quartiers</t>
+  </si>
+  <si>
+    <t>TEST DE LA REINITIALISATION DU JOUEUR</t>
+  </si>
+  <si>
+    <t>le joueur a bien été réinitialisé et toutes les vaeurs sont par défaut</t>
+  </si>
+  <si>
+    <t>TEST DU CONSTRUCTEUR</t>
+  </si>
+  <si>
+    <t>TEST DE L'ATTRIBUTION D'UN JOUEUR</t>
+  </si>
+  <si>
+    <t>le joueur a été bien attribué et les valeurs sont correctes</t>
+  </si>
+  <si>
+    <t>TEST DE LA PERCEPTION DE PIECES D'OR</t>
+  </si>
+  <si>
+    <t>Le nombre pièce doit être changé</t>
+  </si>
+  <si>
+    <t>TEST DE L'AJOUT DE QUARTIER DANS LA MAIN DU JOUEUR</t>
+  </si>
+  <si>
+    <t>Le nombre de quartier dans la main a changé</t>
+  </si>
+  <si>
+    <t>FAIL</t>
+  </si>
+  <si>
+    <t>TEST DE LA CONSTRUCTION D'UN QUARTIER DANS LA CITE DU JOUEUR</t>
+  </si>
+  <si>
+    <t>la cité du joueur a été modifiéé</t>
+  </si>
+  <si>
+    <t>TestQuartier.test8()</t>
+  </si>
+  <si>
+    <t>TestQuartier.test9()</t>
+  </si>
+  <si>
+    <t>TestQuartier.test10()</t>
+  </si>
+  <si>
+    <t>TEST DE LA PERCEPTION DE RESSOURCES SPECIFIQUES</t>
+  </si>
+  <si>
+    <t>le nombre de pièce d'or a été modifé</t>
+  </si>
+  <si>
+    <t xml:space="preserve">FAIL </t>
+  </si>
+  <si>
+    <t>TEST DE L'UTILISATION DU POUVOIR DU ROI</t>
+  </si>
+  <si>
+    <t>TEST DE LA REINITIALISATION</t>
+  </si>
+  <si>
+    <t>le roi a bien été réinitialisé et toutes les valeurs sont par défaut</t>
+  </si>
+  <si>
+    <t>le joueur possède la couronne</t>
+  </si>
+  <si>
+    <t>TestMagicienne.test1()</t>
+  </si>
+  <si>
+    <t>TestMagicienne.test2()</t>
+  </si>
+  <si>
+    <t>tous les champs sont bien initialisés</t>
+  </si>
+  <si>
+    <t>TEST DU POUVOIR DE LA MAGICIENNE</t>
+  </si>
+  <si>
+    <t>taille inchangée de la pioche</t>
   </si>
 </sst>
 </file>
@@ -829,8 +922,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:K26"/>
   <sheetViews>
-    <sheetView topLeftCell="B2" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3:J9"/>
+    <sheetView topLeftCell="D2" workbookViewId="0">
+      <selection activeCell="B3" sqref="B2:K9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1305,19 +1398,19 @@
   <dimension ref="B1:K26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+      <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="21.5703125" customWidth="1"/>
     <col min="3" max="3" width="19.7109375" customWidth="1"/>
-    <col min="4" max="4" width="23.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="26.85546875" customWidth="1"/>
     <col min="5" max="5" width="13.5703125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="7.42578125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="31" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="5" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="7.42578125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="14.7109375" customWidth="1"/>
+    <col min="9" max="9" width="14.28515625" customWidth="1"/>
     <col min="10" max="10" width="27.85546875" customWidth="1"/>
     <col min="11" max="11" width="59.28515625" customWidth="1"/>
   </cols>
@@ -1362,13 +1455,27 @@
       <c r="C3" s="15" t="s">
         <v>33</v>
       </c>
-      <c r="D3" s="9"/>
-      <c r="E3" s="9"/>
-      <c r="F3" s="9"/>
-      <c r="G3" s="9"/>
-      <c r="H3" s="9"/>
-      <c r="I3" s="9"/>
-      <c r="J3" s="9"/>
+      <c r="D3" s="9" t="s">
+        <v>40</v>
+      </c>
+      <c r="E3" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="F3" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="G3" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="H3" s="19">
+        <v>44516</v>
+      </c>
+      <c r="I3" s="9" t="s">
+        <v>38</v>
+      </c>
+      <c r="J3" s="9" t="s">
+        <v>39</v>
+      </c>
       <c r="K3" s="10"/>
     </row>
     <row r="4" spans="2:11" x14ac:dyDescent="0.25">
@@ -1378,13 +1485,27 @@
       <c r="C4" s="15" t="s">
         <v>34</v>
       </c>
-      <c r="D4" s="18"/>
-      <c r="E4" s="9"/>
-      <c r="F4" s="9"/>
-      <c r="G4" s="9"/>
-      <c r="H4" s="2"/>
-      <c r="I4" s="2"/>
-      <c r="J4" s="2"/>
+      <c r="D4" s="18" t="s">
+        <v>46</v>
+      </c>
+      <c r="E4" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="F4" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="G4" s="9" t="s">
+        <v>47</v>
+      </c>
+      <c r="H4" s="19">
+        <v>44516</v>
+      </c>
+      <c r="I4" s="9" t="s">
+        <v>38</v>
+      </c>
+      <c r="J4" s="9" t="s">
+        <v>39</v>
+      </c>
       <c r="K4" s="4"/>
     </row>
     <row r="5" spans="2:11" x14ac:dyDescent="0.25">
@@ -1394,13 +1515,27 @@
       <c r="C5" s="15" t="s">
         <v>35</v>
       </c>
-      <c r="D5" s="18"/>
-      <c r="E5" s="9"/>
-      <c r="F5" s="9"/>
-      <c r="G5" s="9"/>
-      <c r="H5" s="2"/>
-      <c r="I5" s="2"/>
-      <c r="J5" s="2"/>
+      <c r="D5" s="18" t="s">
+        <v>48</v>
+      </c>
+      <c r="E5" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="F5" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="G5" s="9" t="s">
+        <v>49</v>
+      </c>
+      <c r="H5" s="19">
+        <v>44516</v>
+      </c>
+      <c r="I5" s="9" t="s">
+        <v>38</v>
+      </c>
+      <c r="J5" s="9" t="s">
+        <v>39</v>
+      </c>
       <c r="K5" s="4"/>
     </row>
     <row r="6" spans="2:11" x14ac:dyDescent="0.25">
@@ -1410,13 +1545,27 @@
       <c r="C6" s="15" t="s">
         <v>36</v>
       </c>
-      <c r="D6" s="18"/>
-      <c r="E6" s="9"/>
-      <c r="F6" s="9"/>
-      <c r="G6" s="9"/>
-      <c r="H6" s="2"/>
-      <c r="I6" s="2"/>
-      <c r="J6" s="2"/>
+      <c r="D6" s="18" t="s">
+        <v>50</v>
+      </c>
+      <c r="E6" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="F6" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="G6" s="9" t="s">
+        <v>51</v>
+      </c>
+      <c r="H6" s="19">
+        <v>44517</v>
+      </c>
+      <c r="I6" s="9" t="s">
+        <v>38</v>
+      </c>
+      <c r="J6" s="9" t="s">
+        <v>39</v>
+      </c>
       <c r="K6" s="4"/>
     </row>
     <row r="7" spans="2:11" x14ac:dyDescent="0.25">
@@ -1426,13 +1575,27 @@
       <c r="C7" s="15" t="s">
         <v>37</v>
       </c>
-      <c r="D7" s="18"/>
-      <c r="E7" s="9"/>
-      <c r="F7" s="9"/>
-      <c r="G7" s="9"/>
-      <c r="H7" s="2"/>
-      <c r="I7" s="2"/>
-      <c r="J7" s="2"/>
+      <c r="D7" s="18" t="s">
+        <v>52</v>
+      </c>
+      <c r="E7" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="F7" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="G7" s="9" t="s">
+        <v>53</v>
+      </c>
+      <c r="H7" s="19">
+        <v>44517</v>
+      </c>
+      <c r="I7" s="9" t="s">
+        <v>38</v>
+      </c>
+      <c r="J7" s="9" t="s">
+        <v>39</v>
+      </c>
       <c r="K7" s="4"/>
     </row>
     <row r="8" spans="2:11" x14ac:dyDescent="0.25">
@@ -1672,15 +1835,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:K26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G6" sqref="G6"/>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="J25" sqref="J25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="21.140625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="19.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="31.7109375" customWidth="1"/>
+    <col min="4" max="4" width="36.42578125" customWidth="1"/>
     <col min="5" max="5" width="13.5703125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="7.42578125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="31.28515625" customWidth="1"/>
@@ -1730,7 +1893,7 @@
         <v>14</v>
       </c>
       <c r="D3" s="9" t="s">
-        <v>40</v>
+        <v>54</v>
       </c>
       <c r="E3" s="9" t="s">
         <v>10</v>
@@ -1742,7 +1905,7 @@
         <v>41</v>
       </c>
       <c r="H3" s="19">
-        <v>44515</v>
+        <v>44519</v>
       </c>
       <c r="I3" s="9" t="s">
         <v>38</v>
@@ -1760,7 +1923,7 @@
         <v>15</v>
       </c>
       <c r="D4" s="18" t="s">
-        <v>42</v>
+        <v>55</v>
       </c>
       <c r="E4" s="9" t="s">
         <v>10</v>
@@ -1769,10 +1932,10 @@
         <v>10</v>
       </c>
       <c r="G4" s="9" t="s">
-        <v>43</v>
+        <v>56</v>
       </c>
       <c r="H4" s="19">
-        <v>44515</v>
+        <v>44519</v>
       </c>
       <c r="I4" s="9" t="s">
         <v>38</v>
@@ -1790,7 +1953,7 @@
         <v>18</v>
       </c>
       <c r="D5" s="18" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="E5" s="9" t="s">
         <v>10</v>
@@ -1799,10 +1962,10 @@
         <v>10</v>
       </c>
       <c r="G5" s="9" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="H5" s="19">
-        <v>44515</v>
+        <v>44519</v>
       </c>
       <c r="I5" s="9" t="s">
         <v>38</v>
@@ -1820,7 +1983,7 @@
         <v>21</v>
       </c>
       <c r="D6" s="18" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="E6" s="9" t="s">
         <v>10</v>
@@ -1829,10 +1992,10 @@
         <v>10</v>
       </c>
       <c r="G6" s="9" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="H6" s="19">
-        <v>44515</v>
+        <v>44519</v>
       </c>
       <c r="I6" s="9" t="s">
         <v>38</v>
@@ -1850,7 +2013,7 @@
         <v>22</v>
       </c>
       <c r="D7" s="18" t="s">
-        <v>23</v>
+        <v>57</v>
       </c>
       <c r="E7" s="9" t="s">
         <v>10</v>
@@ -1859,10 +2022,10 @@
         <v>10</v>
       </c>
       <c r="G7" s="9" t="s">
-        <v>17</v>
+        <v>58</v>
       </c>
       <c r="H7" s="19">
-        <v>44515</v>
+        <v>44519</v>
       </c>
       <c r="I7" s="9" t="s">
         <v>38</v>
@@ -1880,7 +2043,7 @@
         <v>24</v>
       </c>
       <c r="D8" s="18" t="s">
-        <v>25</v>
+        <v>59</v>
       </c>
       <c r="E8" s="9" t="s">
         <v>10</v>
@@ -1889,16 +2052,16 @@
         <v>10</v>
       </c>
       <c r="G8" s="9" t="s">
-        <v>17</v>
+        <v>60</v>
       </c>
       <c r="H8" s="19">
-        <v>44515</v>
+        <v>44520</v>
       </c>
       <c r="I8" s="9" t="s">
         <v>38</v>
       </c>
       <c r="J8" s="9" t="s">
-        <v>39</v>
+        <v>61</v>
       </c>
       <c r="K8" s="4"/>
     </row>
@@ -1907,233 +2070,503 @@
         <v>9</v>
       </c>
       <c r="C9" s="15" t="s">
+        <v>24</v>
+      </c>
+      <c r="D9" s="18" t="s">
+        <v>59</v>
+      </c>
+      <c r="E9" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="F9" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="G9" s="9" t="s">
+        <v>60</v>
+      </c>
+      <c r="H9" s="19">
+        <v>44520</v>
+      </c>
+      <c r="I9" s="9" t="s">
+        <v>38</v>
+      </c>
+      <c r="J9" s="9" t="s">
+        <v>61</v>
+      </c>
+      <c r="K9" s="4"/>
+    </row>
+    <row r="10" spans="2:11" ht="30" x14ac:dyDescent="0.25">
+      <c r="B10" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="C10" s="15" t="s">
+        <v>24</v>
+      </c>
+      <c r="D10" s="18" t="s">
+        <v>59</v>
+      </c>
+      <c r="E10" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="F10" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="G10" s="9" t="s">
+        <v>60</v>
+      </c>
+      <c r="H10" s="19">
+        <v>44521</v>
+      </c>
+      <c r="I10" s="9" t="s">
+        <v>38</v>
+      </c>
+      <c r="J10" s="9" t="s">
+        <v>61</v>
+      </c>
+      <c r="K10" s="4"/>
+    </row>
+    <row r="11" spans="2:11" ht="30" x14ac:dyDescent="0.25">
+      <c r="B11" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="C11" s="15" t="s">
+        <v>24</v>
+      </c>
+      <c r="D11" s="18" t="s">
+        <v>59</v>
+      </c>
+      <c r="E11" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="F11" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="G11" s="9" t="s">
+        <v>60</v>
+      </c>
+      <c r="H11" s="19">
+        <v>44521</v>
+      </c>
+      <c r="I11" s="9" t="s">
+        <v>38</v>
+      </c>
+      <c r="J11" s="9" t="s">
+        <v>39</v>
+      </c>
+      <c r="K11" s="4"/>
+    </row>
+    <row r="12" spans="2:11" ht="30" x14ac:dyDescent="0.25">
+      <c r="B12" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="C12" s="15" t="s">
         <v>26</v>
       </c>
-      <c r="D9" s="18" t="s">
-        <v>27</v>
-      </c>
-      <c r="E9" s="9" t="s">
-        <v>10</v>
-      </c>
-      <c r="F9" s="9" t="s">
-        <v>10</v>
-      </c>
-      <c r="G9" s="18" t="s">
-        <v>28</v>
-      </c>
-      <c r="H9" s="19">
-        <v>44515</v>
-      </c>
-      <c r="I9" s="9" t="s">
-        <v>38</v>
-      </c>
-      <c r="J9" s="9" t="s">
+      <c r="D12" s="18" t="s">
+        <v>62</v>
+      </c>
+      <c r="E12" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="F12" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="G12" s="18" t="s">
+        <v>63</v>
+      </c>
+      <c r="H12" s="19">
+        <v>44521</v>
+      </c>
+      <c r="I12" s="9" t="s">
+        <v>38</v>
+      </c>
+      <c r="J12" s="9" t="s">
+        <v>61</v>
+      </c>
+      <c r="K12" s="4"/>
+    </row>
+    <row r="13" spans="2:11" ht="30" x14ac:dyDescent="0.25">
+      <c r="B13" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="C13" s="15" t="s">
+        <v>26</v>
+      </c>
+      <c r="D13" s="18" t="s">
+        <v>62</v>
+      </c>
+      <c r="E13" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="F13" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="G13" s="18" t="s">
+        <v>63</v>
+      </c>
+      <c r="H13" s="19">
+        <v>44521</v>
+      </c>
+      <c r="I13" s="9" t="s">
+        <v>38</v>
+      </c>
+      <c r="J13" s="9" t="s">
+        <v>61</v>
+      </c>
+      <c r="K13" s="4"/>
+    </row>
+    <row r="14" spans="2:11" ht="30" x14ac:dyDescent="0.25">
+      <c r="B14" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="C14" s="15" t="s">
+        <v>26</v>
+      </c>
+      <c r="D14" s="18" t="s">
+        <v>62</v>
+      </c>
+      <c r="E14" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="F14" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="G14" s="18" t="s">
+        <v>63</v>
+      </c>
+      <c r="H14" s="19">
+        <v>44522</v>
+      </c>
+      <c r="I14" s="9" t="s">
+        <v>38</v>
+      </c>
+      <c r="J14" s="9" t="s">
+        <v>61</v>
+      </c>
+      <c r="K14" s="4"/>
+    </row>
+    <row r="15" spans="2:11" ht="30" x14ac:dyDescent="0.25">
+      <c r="B15" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="C15" s="15" t="s">
+        <v>26</v>
+      </c>
+      <c r="D15" s="18" t="s">
+        <v>62</v>
+      </c>
+      <c r="E15" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="F15" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="G15" s="18" t="s">
+        <v>63</v>
+      </c>
+      <c r="H15" s="19">
+        <v>44522</v>
+      </c>
+      <c r="I15" s="9" t="s">
+        <v>38</v>
+      </c>
+      <c r="J15" s="9" t="s">
         <v>39</v>
       </c>
-      <c r="K9" s="4"/>
-    </row>
-    <row r="10" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B10" s="3"/>
-      <c r="C10" s="16"/>
-      <c r="D10" s="2"/>
-      <c r="E10" s="2"/>
-      <c r="F10" s="2"/>
-      <c r="G10" s="2"/>
-      <c r="H10" s="2"/>
-      <c r="I10" s="2"/>
-      <c r="J10" s="2"/>
-      <c r="K10" s="4"/>
-    </row>
-    <row r="11" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B11" s="3"/>
-      <c r="C11" s="16"/>
-      <c r="D11" s="2"/>
-      <c r="E11" s="2"/>
-      <c r="F11" s="2"/>
-      <c r="G11" s="2"/>
-      <c r="H11" s="2"/>
-      <c r="I11" s="2"/>
-      <c r="J11" s="2"/>
-      <c r="K11" s="4"/>
-    </row>
-    <row r="12" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B12" s="3"/>
-      <c r="C12" s="16"/>
-      <c r="D12" s="2"/>
-      <c r="E12" s="2"/>
-      <c r="F12" s="2"/>
-      <c r="G12" s="2"/>
-      <c r="H12" s="2"/>
-      <c r="I12" s="2"/>
-      <c r="J12" s="2"/>
-      <c r="K12" s="4"/>
-    </row>
-    <row r="13" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B13" s="3"/>
-      <c r="C13" s="16"/>
-      <c r="D13" s="2"/>
-      <c r="E13" s="2"/>
-      <c r="F13" s="2"/>
-      <c r="G13" s="2"/>
-      <c r="H13" s="2"/>
-      <c r="I13" s="2"/>
-      <c r="J13" s="2"/>
-      <c r="K13" s="4"/>
-    </row>
-    <row r="14" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B14" s="3"/>
-      <c r="C14" s="16"/>
-      <c r="D14" s="2"/>
-      <c r="E14" s="2"/>
-      <c r="F14" s="2"/>
-      <c r="G14" s="2"/>
-      <c r="H14" s="2"/>
-      <c r="I14" s="2"/>
-      <c r="J14" s="2"/>
-      <c r="K14" s="4"/>
-    </row>
-    <row r="15" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B15" s="3"/>
-      <c r="C15" s="16"/>
-      <c r="D15" s="2"/>
-      <c r="E15" s="2"/>
-      <c r="F15" s="2"/>
-      <c r="G15" s="2"/>
-      <c r="H15" s="2"/>
-      <c r="I15" s="2"/>
-      <c r="J15" s="2"/>
       <c r="K15" s="4"/>
     </row>
-    <row r="16" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B16" s="3"/>
-      <c r="C16" s="16"/>
-      <c r="D16" s="2"/>
-      <c r="E16" s="2"/>
-      <c r="F16" s="2"/>
-      <c r="G16" s="2"/>
-      <c r="H16" s="2"/>
-      <c r="I16" s="2"/>
-      <c r="J16" s="2"/>
+    <row r="16" spans="2:11" ht="30" x14ac:dyDescent="0.25">
+      <c r="B16" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="C16" s="15" t="s">
+        <v>26</v>
+      </c>
+      <c r="D16" s="18" t="s">
+        <v>62</v>
+      </c>
+      <c r="E16" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="F16" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="G16" s="18" t="s">
+        <v>63</v>
+      </c>
+      <c r="H16" s="19">
+        <v>44523</v>
+      </c>
+      <c r="I16" s="9" t="s">
+        <v>38</v>
+      </c>
+      <c r="J16" s="9" t="s">
+        <v>39</v>
+      </c>
       <c r="K16" s="4"/>
     </row>
-    <row r="17" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B17" s="3"/>
-      <c r="C17" s="16"/>
-      <c r="D17" s="2"/>
-      <c r="E17" s="2"/>
-      <c r="F17" s="2"/>
-      <c r="G17" s="2"/>
-      <c r="H17" s="2"/>
-      <c r="I17" s="2"/>
-      <c r="J17" s="2"/>
+    <row r="17" spans="2:11" ht="30" x14ac:dyDescent="0.25">
+      <c r="B17" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="C17" s="15" t="s">
+        <v>64</v>
+      </c>
+      <c r="D17" s="18" t="s">
+        <v>67</v>
+      </c>
+      <c r="E17" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="F17" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="G17" s="18" t="s">
+        <v>68</v>
+      </c>
+      <c r="H17" s="19">
+        <v>44523</v>
+      </c>
+      <c r="I17" s="9" t="s">
+        <v>38</v>
+      </c>
+      <c r="J17" s="9" t="s">
+        <v>61</v>
+      </c>
       <c r="K17" s="4"/>
     </row>
-    <row r="18" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B18" s="3"/>
-      <c r="C18" s="16"/>
-      <c r="D18" s="2"/>
-      <c r="E18" s="2"/>
-      <c r="F18" s="2"/>
-      <c r="G18" s="2"/>
-      <c r="H18" s="2"/>
-      <c r="I18" s="2"/>
-      <c r="J18" s="2"/>
+    <row r="18" spans="2:11" ht="30" x14ac:dyDescent="0.25">
+      <c r="B18" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="C18" s="15" t="s">
+        <v>64</v>
+      </c>
+      <c r="D18" s="18" t="s">
+        <v>67</v>
+      </c>
+      <c r="E18" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="F18" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="G18" s="18" t="s">
+        <v>68</v>
+      </c>
+      <c r="H18" s="19">
+        <v>44523</v>
+      </c>
+      <c r="I18" s="9" t="s">
+        <v>38</v>
+      </c>
+      <c r="J18" s="9" t="s">
+        <v>61</v>
+      </c>
       <c r="K18" s="4"/>
     </row>
-    <row r="19" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B19" s="3"/>
-      <c r="C19" s="16"/>
-      <c r="D19" s="2"/>
-      <c r="E19" s="2"/>
-      <c r="F19" s="2"/>
-      <c r="G19" s="2"/>
-      <c r="H19" s="2"/>
-      <c r="I19" s="2"/>
-      <c r="J19" s="2"/>
+    <row r="19" spans="2:11" ht="30" x14ac:dyDescent="0.25">
+      <c r="B19" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="C19" s="15" t="s">
+        <v>64</v>
+      </c>
+      <c r="D19" s="18" t="s">
+        <v>67</v>
+      </c>
+      <c r="E19" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="F19" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="G19" s="18" t="s">
+        <v>68</v>
+      </c>
+      <c r="H19" s="19">
+        <v>44523</v>
+      </c>
+      <c r="I19" s="9" t="s">
+        <v>38</v>
+      </c>
+      <c r="J19" s="9" t="s">
+        <v>61</v>
+      </c>
       <c r="K19" s="4"/>
     </row>
-    <row r="20" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B20" s="3"/>
-      <c r="C20" s="16"/>
-      <c r="D20" s="2"/>
-      <c r="E20" s="2"/>
-      <c r="F20" s="2"/>
-      <c r="G20" s="2"/>
-      <c r="H20" s="2"/>
-      <c r="I20" s="2"/>
-      <c r="J20" s="2"/>
+    <row r="20" spans="2:11" ht="30" x14ac:dyDescent="0.25">
+      <c r="B20" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="C20" s="15" t="s">
+        <v>64</v>
+      </c>
+      <c r="D20" s="18" t="s">
+        <v>67</v>
+      </c>
+      <c r="E20" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="F20" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="G20" s="18" t="s">
+        <v>68</v>
+      </c>
+      <c r="H20" s="19">
+        <v>44524</v>
+      </c>
+      <c r="I20" s="9" t="s">
+        <v>38</v>
+      </c>
+      <c r="J20" s="9" t="s">
+        <v>61</v>
+      </c>
       <c r="K20" s="4"/>
     </row>
-    <row r="21" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B21" s="3"/>
-      <c r="C21" s="16"/>
-      <c r="D21" s="2"/>
-      <c r="E21" s="2"/>
-      <c r="F21" s="2"/>
-      <c r="G21" s="2"/>
-      <c r="H21" s="2"/>
-      <c r="I21" s="2"/>
-      <c r="J21" s="2"/>
+    <row r="21" spans="2:11" ht="30" x14ac:dyDescent="0.25">
+      <c r="B21" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="C21" s="15" t="s">
+        <v>64</v>
+      </c>
+      <c r="D21" s="18" t="s">
+        <v>67</v>
+      </c>
+      <c r="E21" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="F21" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="G21" s="18" t="s">
+        <v>68</v>
+      </c>
+      <c r="H21" s="19">
+        <v>44524</v>
+      </c>
+      <c r="I21" s="9" t="s">
+        <v>38</v>
+      </c>
+      <c r="J21" s="9" t="s">
+        <v>39</v>
+      </c>
       <c r="K21" s="4"/>
     </row>
-    <row r="22" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B22" s="3"/>
-      <c r="C22" s="16"/>
-      <c r="D22" s="2"/>
-      <c r="E22" s="2"/>
-      <c r="F22" s="2"/>
-      <c r="G22" s="2"/>
-      <c r="H22" s="2"/>
-      <c r="I22" s="2"/>
-      <c r="J22" s="2"/>
+    <row r="22" spans="2:11" ht="30" x14ac:dyDescent="0.25">
+      <c r="B22" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="C22" s="15" t="s">
+        <v>65</v>
+      </c>
+      <c r="D22" s="18" t="s">
+        <v>70</v>
+      </c>
+      <c r="E22" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="F22" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="G22" s="18" t="s">
+        <v>73</v>
+      </c>
+      <c r="H22" s="19">
+        <v>44524</v>
+      </c>
+      <c r="I22" s="9" t="s">
+        <v>38</v>
+      </c>
+      <c r="J22" s="9" t="s">
+        <v>69</v>
+      </c>
       <c r="K22" s="4"/>
     </row>
-    <row r="23" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B23" s="3"/>
-      <c r="C23" s="16"/>
-      <c r="D23" s="2"/>
-      <c r="E23" s="2"/>
-      <c r="F23" s="2"/>
-      <c r="G23" s="2"/>
-      <c r="H23" s="2"/>
-      <c r="I23" s="2"/>
-      <c r="J23" s="2"/>
+    <row r="23" spans="2:11" ht="30" x14ac:dyDescent="0.25">
+      <c r="B23" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="C23" s="15" t="s">
+        <v>65</v>
+      </c>
+      <c r="D23" s="18" t="s">
+        <v>70</v>
+      </c>
+      <c r="E23" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="F23" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="G23" s="18" t="s">
+        <v>73</v>
+      </c>
+      <c r="H23" s="19">
+        <v>44524</v>
+      </c>
+      <c r="I23" s="9" t="s">
+        <v>38</v>
+      </c>
+      <c r="J23" s="9" t="s">
+        <v>39</v>
+      </c>
       <c r="K23" s="4"/>
     </row>
     <row r="24" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B24" s="3"/>
-      <c r="C24" s="16"/>
-      <c r="D24" s="2"/>
-      <c r="E24" s="2"/>
-      <c r="F24" s="2"/>
-      <c r="G24" s="2"/>
-      <c r="H24" s="2"/>
-      <c r="I24" s="2"/>
-      <c r="J24" s="2"/>
+      <c r="B24" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="C24" s="15" t="s">
+        <v>66</v>
+      </c>
+      <c r="D24" s="18" t="s">
+        <v>71</v>
+      </c>
+      <c r="E24" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="F24" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="G24" s="9" t="s">
+        <v>72</v>
+      </c>
+      <c r="H24" s="19">
+        <v>44554</v>
+      </c>
+      <c r="I24" s="9" t="s">
+        <v>38</v>
+      </c>
+      <c r="J24" s="9" t="s">
+        <v>39</v>
+      </c>
       <c r="K24" s="4"/>
     </row>
     <row r="25" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B25" s="3"/>
-      <c r="C25" s="16"/>
-      <c r="D25" s="2"/>
-      <c r="E25" s="2"/>
-      <c r="F25" s="2"/>
-      <c r="G25" s="2"/>
-      <c r="H25" s="2"/>
-      <c r="I25" s="2"/>
-      <c r="J25" s="2"/>
+      <c r="B25" s="8"/>
+      <c r="C25" s="15"/>
+      <c r="D25" s="18"/>
+      <c r="E25" s="9"/>
+      <c r="F25" s="9"/>
+      <c r="G25" s="18"/>
+      <c r="H25" s="19"/>
+      <c r="I25" s="9"/>
+      <c r="J25" s="9"/>
       <c r="K25" s="4"/>
     </row>
     <row r="26" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B26" s="5"/>
-      <c r="C26" s="17"/>
-      <c r="D26" s="6"/>
-      <c r="E26" s="6"/>
-      <c r="F26" s="6"/>
-      <c r="G26" s="6"/>
-      <c r="H26" s="6"/>
-      <c r="I26" s="6"/>
-      <c r="J26" s="6"/>
+      <c r="B26" s="8"/>
+      <c r="C26" s="15"/>
+      <c r="D26" s="18"/>
+      <c r="E26" s="9"/>
+      <c r="F26" s="9"/>
+      <c r="G26" s="18"/>
+      <c r="H26" s="19"/>
+      <c r="I26" s="9"/>
+      <c r="J26" s="9"/>
       <c r="K26" s="7"/>
     </row>
   </sheetData>
@@ -2177,4 +2610,234 @@
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:J8"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I6" sqref="I6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="18.7109375" customWidth="1"/>
+    <col min="2" max="2" width="21.7109375" customWidth="1"/>
+    <col min="3" max="3" width="35.5703125" customWidth="1"/>
+    <col min="4" max="4" width="18.140625" customWidth="1"/>
+    <col min="5" max="5" width="17.42578125" customWidth="1"/>
+    <col min="6" max="6" width="33.140625" customWidth="1"/>
+    <col min="7" max="8" width="14.28515625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" ht="75.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="B1" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="C1" s="12" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1" s="12" t="s">
+        <v>1</v>
+      </c>
+      <c r="E1" s="12" t="s">
+        <v>2</v>
+      </c>
+      <c r="F1" s="12" t="s">
+        <v>3</v>
+      </c>
+      <c r="G1" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="H1" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="I1" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="J1" s="14" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A2" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="B2" s="15" t="s">
+        <v>74</v>
+      </c>
+      <c r="C2" s="9" t="s">
+        <v>54</v>
+      </c>
+      <c r="D2" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="E2" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="F2" s="9" t="s">
+        <v>76</v>
+      </c>
+      <c r="G2" s="19">
+        <v>44504</v>
+      </c>
+      <c r="H2" s="9" t="s">
+        <v>38</v>
+      </c>
+      <c r="I2" s="9" t="s">
+        <v>39</v>
+      </c>
+      <c r="J2" s="10"/>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A3" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3" s="15" t="s">
+        <v>75</v>
+      </c>
+      <c r="C3" s="18" t="s">
+        <v>77</v>
+      </c>
+      <c r="D3" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="E3" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="F3" s="9" t="s">
+        <v>78</v>
+      </c>
+      <c r="G3" s="19">
+        <v>44504</v>
+      </c>
+      <c r="H3" s="9" t="s">
+        <v>38</v>
+      </c>
+      <c r="I3" s="9" t="s">
+        <v>61</v>
+      </c>
+      <c r="J3" s="4"/>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A4" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="B4" s="15" t="s">
+        <v>75</v>
+      </c>
+      <c r="C4" s="18" t="s">
+        <v>77</v>
+      </c>
+      <c r="D4" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="E4" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="F4" s="9" t="s">
+        <v>78</v>
+      </c>
+      <c r="G4" s="19">
+        <v>44504</v>
+      </c>
+      <c r="H4" s="9" t="s">
+        <v>38</v>
+      </c>
+      <c r="I4" s="9" t="s">
+        <v>61</v>
+      </c>
+      <c r="J4" s="4"/>
+    </row>
+    <row r="5" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="A5" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="B5" s="15" t="s">
+        <v>75</v>
+      </c>
+      <c r="C5" s="18" t="s">
+        <v>77</v>
+      </c>
+      <c r="D5" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="E5" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="F5" s="9" t="s">
+        <v>78</v>
+      </c>
+      <c r="G5" s="19">
+        <v>44504</v>
+      </c>
+      <c r="H5" s="9" t="s">
+        <v>38</v>
+      </c>
+      <c r="I5" s="9" t="s">
+        <v>61</v>
+      </c>
+      <c r="J5" s="4"/>
+    </row>
+    <row r="6" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="A6" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="B6" s="15" t="s">
+        <v>75</v>
+      </c>
+      <c r="C6" s="18" t="s">
+        <v>77</v>
+      </c>
+      <c r="D6" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="E6" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="F6" s="9" t="s">
+        <v>78</v>
+      </c>
+      <c r="G6" s="19">
+        <v>44504</v>
+      </c>
+      <c r="H6" s="9" t="s">
+        <v>38</v>
+      </c>
+      <c r="I6" s="9" t="s">
+        <v>39</v>
+      </c>
+      <c r="J6" s="4"/>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A7" s="8"/>
+      <c r="B7" s="15"/>
+      <c r="C7" s="18"/>
+      <c r="D7" s="9"/>
+      <c r="E7" s="9"/>
+      <c r="F7" s="9"/>
+      <c r="G7" s="19"/>
+      <c r="H7" s="9"/>
+      <c r="I7" s="9"/>
+      <c r="J7" s="4"/>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A8" s="8"/>
+      <c r="B8" s="15"/>
+      <c r="C8" s="18"/>
+      <c r="D8" s="9"/>
+      <c r="E8" s="9"/>
+      <c r="F8" s="18"/>
+      <c r="G8" s="19"/>
+      <c r="H8" s="9"/>
+      <c r="I8" s="9"/>
+      <c r="J8" s="4"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
add tests class joueur
</commit_message>
<xml_diff>
--- a/src/ressources/cahierDeTests.xlsx
+++ b/src/ressources/cahierDeTests.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24701"/>
+  <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\HP\eclipse-2021-workspace\Citadelle\src\ressources\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\askri\git\Citadelle\src\ressources\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C4B23CAA-6033-4324-938F-81B1207B7265}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="11430" windowHeight="3765" firstSheet="3" activeTab="7"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" firstSheet="3" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Objectifs" sheetId="1" r:id="rId1"/>
@@ -26,21 +27,12 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="356" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="396" uniqueCount="91">
   <si>
     <t>Objectif</t>
   </si>
@@ -287,12 +279,48 @@
   </si>
   <si>
     <t>taille inchangée de la pioche</t>
+  </si>
+  <si>
+    <t>testJoueur.test1();</t>
+  </si>
+  <si>
+    <t>Razi Askri</t>
+  </si>
+  <si>
+    <t>Passed</t>
+  </si>
+  <si>
+    <t>test du nom du joueur, test du trésor initial du joueur, test de nombre de quartiers dans la cite, test du nombre de quartiers dans la main du joueur.</t>
+  </si>
+  <si>
+    <t>testJoueur.test2();</t>
+  </si>
+  <si>
+    <t>test de l'ajout d'un nombre de pièces, test d'ajout d'un nombre de pièces négatif, test d'un retrait d'un nombre négatif de pièces, test de retrait d'un trop grand nombre de pièces, test de retrait d'un nombre de pièces.</t>
+  </si>
+  <si>
+    <t>testJoueur.test3();</t>
+  </si>
+  <si>
+    <t xml:space="preserve">test de l'ajout de trois quartiers, test de présence d'un quartier, test de retrait d'un quartier, test de non présence d'un quartier. </t>
+  </si>
+  <si>
+    <t>testJoueur.test4();</t>
+  </si>
+  <si>
+    <t xml:space="preserve">test de l'ajout de trois quartiers, test de retrait d'un quartier. </t>
+  </si>
+  <si>
+    <t>testJoueur.test5();</t>
+  </si>
+  <si>
+    <t>test de la réinitialisation</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -316,7 +344,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="16">
+  <borders count="18">
     <border>
       <left/>
       <right/>
@@ -535,11 +563,33 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -568,6 +618,33 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -881,34 +958,34 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B2:B5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="77.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="77.26953125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:2" ht="45" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:2" ht="43.5" x14ac:dyDescent="0.35">
       <c r="B2" s="1" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="3" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B3" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="4" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B4" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="5" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B5" t="s">
         <v>31</v>
       </c>
@@ -919,30 +996,30 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="B1:K26"/>
   <sheetViews>
     <sheetView topLeftCell="D2" workbookViewId="0">
       <selection activeCell="B3" sqref="B2:K9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="3.5703125" customWidth="1"/>
-    <col min="2" max="2" width="20.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="18.140625" customWidth="1"/>
-    <col min="4" max="4" width="27.7109375" customWidth="1"/>
-    <col min="5" max="5" width="12.7109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="8.85546875" customWidth="1"/>
+    <col min="1" max="1" width="3.54296875" customWidth="1"/>
+    <col min="2" max="2" width="20.7265625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.1796875" customWidth="1"/>
+    <col min="4" max="4" width="27.7265625" customWidth="1"/>
+    <col min="5" max="5" width="12.7265625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="8.81640625" customWidth="1"/>
     <col min="7" max="7" width="31" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="11.7109375" customWidth="1"/>
-    <col min="9" max="9" width="9.140625" customWidth="1"/>
-    <col min="10" max="10" width="21.42578125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="48.140625" customWidth="1"/>
+    <col min="8" max="8" width="11.7265625" customWidth="1"/>
+    <col min="9" max="9" width="9.1796875" customWidth="1"/>
+    <col min="10" max="10" width="21.453125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="48.1796875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="2" spans="2:11" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="2:11" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
+    <row r="2" spans="2:11" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B2" s="11" t="s">
         <v>13</v>
       </c>
@@ -974,7 +1051,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:11" x14ac:dyDescent="0.35">
       <c r="B3" s="8" t="s">
         <v>9</v>
       </c>
@@ -1004,7 +1081,7 @@
       </c>
       <c r="K3" s="10"/>
     </row>
-    <row r="4" spans="2:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:11" ht="29" x14ac:dyDescent="0.35">
       <c r="B4" s="8" t="s">
         <v>9</v>
       </c>
@@ -1034,7 +1111,7 @@
       </c>
       <c r="K4" s="4"/>
     </row>
-    <row r="5" spans="2:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:11" ht="29" x14ac:dyDescent="0.35">
       <c r="B5" s="8" t="s">
         <v>9</v>
       </c>
@@ -1064,7 +1141,7 @@
       </c>
       <c r="K5" s="4"/>
     </row>
-    <row r="6" spans="2:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:11" ht="29" x14ac:dyDescent="0.35">
       <c r="B6" s="8" t="s">
         <v>9</v>
       </c>
@@ -1094,7 +1171,7 @@
       </c>
       <c r="K6" s="4"/>
     </row>
-    <row r="7" spans="2:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:11" ht="29" x14ac:dyDescent="0.35">
       <c r="B7" s="8" t="s">
         <v>9</v>
       </c>
@@ -1124,7 +1201,7 @@
       </c>
       <c r="K7" s="4"/>
     </row>
-    <row r="8" spans="2:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:11" ht="29" x14ac:dyDescent="0.35">
       <c r="B8" s="8" t="s">
         <v>9</v>
       </c>
@@ -1154,7 +1231,7 @@
       </c>
       <c r="K8" s="4"/>
     </row>
-    <row r="9" spans="2:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:11" ht="29" x14ac:dyDescent="0.35">
       <c r="B9" s="8" t="s">
         <v>9</v>
       </c>
@@ -1184,7 +1261,7 @@
       </c>
       <c r="K9" s="4"/>
     </row>
-    <row r="10" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:11" x14ac:dyDescent="0.35">
       <c r="B10" s="3"/>
       <c r="C10" s="16"/>
       <c r="D10" s="2"/>
@@ -1196,7 +1273,7 @@
       <c r="J10" s="2"/>
       <c r="K10" s="4"/>
     </row>
-    <row r="11" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:11" x14ac:dyDescent="0.35">
       <c r="B11" s="3"/>
       <c r="C11" s="16"/>
       <c r="D11" s="2"/>
@@ -1208,7 +1285,7 @@
       <c r="J11" s="2"/>
       <c r="K11" s="4"/>
     </row>
-    <row r="12" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:11" x14ac:dyDescent="0.35">
       <c r="B12" s="3"/>
       <c r="C12" s="16"/>
       <c r="D12" s="2"/>
@@ -1220,7 +1297,7 @@
       <c r="J12" s="2"/>
       <c r="K12" s="4"/>
     </row>
-    <row r="13" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:11" x14ac:dyDescent="0.35">
       <c r="B13" s="3"/>
       <c r="C13" s="16"/>
       <c r="D13" s="2"/>
@@ -1232,7 +1309,7 @@
       <c r="J13" s="2"/>
       <c r="K13" s="4"/>
     </row>
-    <row r="14" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:11" x14ac:dyDescent="0.35">
       <c r="B14" s="3"/>
       <c r="C14" s="16"/>
       <c r="D14" s="2"/>
@@ -1244,7 +1321,7 @@
       <c r="J14" s="2"/>
       <c r="K14" s="4"/>
     </row>
-    <row r="15" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:11" x14ac:dyDescent="0.35">
       <c r="B15" s="3"/>
       <c r="C15" s="16"/>
       <c r="D15" s="2"/>
@@ -1256,7 +1333,7 @@
       <c r="J15" s="2"/>
       <c r="K15" s="4"/>
     </row>
-    <row r="16" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:11" x14ac:dyDescent="0.35">
       <c r="B16" s="3"/>
       <c r="C16" s="16"/>
       <c r="D16" s="2"/>
@@ -1268,7 +1345,7 @@
       <c r="J16" s="2"/>
       <c r="K16" s="4"/>
     </row>
-    <row r="17" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:11" x14ac:dyDescent="0.35">
       <c r="B17" s="3"/>
       <c r="C17" s="16"/>
       <c r="D17" s="2"/>
@@ -1280,7 +1357,7 @@
       <c r="J17" s="2"/>
       <c r="K17" s="4"/>
     </row>
-    <row r="18" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:11" x14ac:dyDescent="0.35">
       <c r="B18" s="3"/>
       <c r="C18" s="16"/>
       <c r="D18" s="2"/>
@@ -1292,7 +1369,7 @@
       <c r="J18" s="2"/>
       <c r="K18" s="4"/>
     </row>
-    <row r="19" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:11" x14ac:dyDescent="0.35">
       <c r="B19" s="3"/>
       <c r="C19" s="16"/>
       <c r="D19" s="2"/>
@@ -1304,7 +1381,7 @@
       <c r="J19" s="2"/>
       <c r="K19" s="4"/>
     </row>
-    <row r="20" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:11" x14ac:dyDescent="0.35">
       <c r="B20" s="3"/>
       <c r="C20" s="16"/>
       <c r="D20" s="2"/>
@@ -1316,7 +1393,7 @@
       <c r="J20" s="2"/>
       <c r="K20" s="4"/>
     </row>
-    <row r="21" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:11" x14ac:dyDescent="0.35">
       <c r="B21" s="3"/>
       <c r="C21" s="16"/>
       <c r="D21" s="2"/>
@@ -1328,7 +1405,7 @@
       <c r="J21" s="2"/>
       <c r="K21" s="4"/>
     </row>
-    <row r="22" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:11" x14ac:dyDescent="0.35">
       <c r="B22" s="3"/>
       <c r="C22" s="16"/>
       <c r="D22" s="2"/>
@@ -1340,7 +1417,7 @@
       <c r="J22" s="2"/>
       <c r="K22" s="4"/>
     </row>
-    <row r="23" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:11" x14ac:dyDescent="0.35">
       <c r="B23" s="3"/>
       <c r="C23" s="16"/>
       <c r="D23" s="2"/>
@@ -1352,7 +1429,7 @@
       <c r="J23" s="2"/>
       <c r="K23" s="4"/>
     </row>
-    <row r="24" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:11" x14ac:dyDescent="0.35">
       <c r="B24" s="3"/>
       <c r="C24" s="16"/>
       <c r="D24" s="2"/>
@@ -1364,7 +1441,7 @@
       <c r="J24" s="2"/>
       <c r="K24" s="4"/>
     </row>
-    <row r="25" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:11" x14ac:dyDescent="0.35">
       <c r="B25" s="3"/>
       <c r="C25" s="16"/>
       <c r="D25" s="2"/>
@@ -1376,7 +1453,7 @@
       <c r="J25" s="2"/>
       <c r="K25" s="4"/>
     </row>
-    <row r="26" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="2:11" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B26" s="5"/>
       <c r="C26" s="17"/>
       <c r="D26" s="6"/>
@@ -1394,29 +1471,29 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="B1:K26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="21.5703125" customWidth="1"/>
-    <col min="3" max="3" width="19.7109375" customWidth="1"/>
-    <col min="4" max="4" width="26.85546875" customWidth="1"/>
-    <col min="5" max="5" width="13.5703125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="7.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="21.54296875" customWidth="1"/>
+    <col min="3" max="3" width="19.7265625" customWidth="1"/>
+    <col min="4" max="4" width="26.81640625" customWidth="1"/>
+    <col min="5" max="5" width="13.54296875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="7.453125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="31" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="14.7109375" customWidth="1"/>
-    <col min="9" max="9" width="14.28515625" customWidth="1"/>
-    <col min="10" max="10" width="27.85546875" customWidth="1"/>
-    <col min="11" max="11" width="59.28515625" customWidth="1"/>
+    <col min="8" max="8" width="14.7265625" customWidth="1"/>
+    <col min="9" max="9" width="14.26953125" customWidth="1"/>
+    <col min="10" max="10" width="27.81640625" customWidth="1"/>
+    <col min="11" max="11" width="59.26953125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="2" spans="2:11" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="2:11" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
+    <row r="2" spans="2:11" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B2" s="11" t="s">
         <v>13</v>
       </c>
@@ -1448,7 +1525,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:11" x14ac:dyDescent="0.35">
       <c r="B3" s="8" t="s">
         <v>9</v>
       </c>
@@ -1478,7 +1555,7 @@
       </c>
       <c r="K3" s="10"/>
     </row>
-    <row r="4" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:11" x14ac:dyDescent="0.35">
       <c r="B4" s="8" t="s">
         <v>9</v>
       </c>
@@ -1508,7 +1585,7 @@
       </c>
       <c r="K4" s="4"/>
     </row>
-    <row r="5" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:11" x14ac:dyDescent="0.35">
       <c r="B5" s="8" t="s">
         <v>9</v>
       </c>
@@ -1538,7 +1615,7 @@
       </c>
       <c r="K5" s="4"/>
     </row>
-    <row r="6" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:11" x14ac:dyDescent="0.35">
       <c r="B6" s="8" t="s">
         <v>9</v>
       </c>
@@ -1568,7 +1645,7 @@
       </c>
       <c r="K6" s="4"/>
     </row>
-    <row r="7" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:11" ht="29" x14ac:dyDescent="0.35">
       <c r="B7" s="8" t="s">
         <v>9</v>
       </c>
@@ -1598,7 +1675,7 @@
       </c>
       <c r="K7" s="4"/>
     </row>
-    <row r="8" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:11" x14ac:dyDescent="0.35">
       <c r="B8" s="8"/>
       <c r="C8" s="15"/>
       <c r="D8" s="18"/>
@@ -1610,7 +1687,7 @@
       <c r="J8" s="2"/>
       <c r="K8" s="4"/>
     </row>
-    <row r="9" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:11" x14ac:dyDescent="0.35">
       <c r="B9" s="8"/>
       <c r="C9" s="15"/>
       <c r="D9" s="18"/>
@@ -1622,7 +1699,7 @@
       <c r="J9" s="2"/>
       <c r="K9" s="4"/>
     </row>
-    <row r="10" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:11" x14ac:dyDescent="0.35">
       <c r="B10" s="3"/>
       <c r="C10" s="16"/>
       <c r="D10" s="2"/>
@@ -1634,7 +1711,7 @@
       <c r="J10" s="2"/>
       <c r="K10" s="4"/>
     </row>
-    <row r="11" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:11" x14ac:dyDescent="0.35">
       <c r="B11" s="3"/>
       <c r="C11" s="16"/>
       <c r="D11" s="2"/>
@@ -1646,7 +1723,7 @@
       <c r="J11" s="2"/>
       <c r="K11" s="4"/>
     </row>
-    <row r="12" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:11" x14ac:dyDescent="0.35">
       <c r="B12" s="3"/>
       <c r="C12" s="16"/>
       <c r="D12" s="2"/>
@@ -1658,7 +1735,7 @@
       <c r="J12" s="2"/>
       <c r="K12" s="4"/>
     </row>
-    <row r="13" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:11" x14ac:dyDescent="0.35">
       <c r="B13" s="3"/>
       <c r="C13" s="16"/>
       <c r="D13" s="2"/>
@@ -1670,7 +1747,7 @@
       <c r="J13" s="2"/>
       <c r="K13" s="4"/>
     </row>
-    <row r="14" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:11" x14ac:dyDescent="0.35">
       <c r="B14" s="3"/>
       <c r="C14" s="16"/>
       <c r="D14" s="2"/>
@@ -1682,7 +1759,7 @@
       <c r="J14" s="2"/>
       <c r="K14" s="4"/>
     </row>
-    <row r="15" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:11" x14ac:dyDescent="0.35">
       <c r="B15" s="3"/>
       <c r="C15" s="16"/>
       <c r="D15" s="2"/>
@@ -1694,7 +1771,7 @@
       <c r="J15" s="2"/>
       <c r="K15" s="4"/>
     </row>
-    <row r="16" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:11" x14ac:dyDescent="0.35">
       <c r="B16" s="3"/>
       <c r="C16" s="16"/>
       <c r="D16" s="2"/>
@@ -1706,7 +1783,7 @@
       <c r="J16" s="2"/>
       <c r="K16" s="4"/>
     </row>
-    <row r="17" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:11" x14ac:dyDescent="0.35">
       <c r="B17" s="3"/>
       <c r="C17" s="16"/>
       <c r="D17" s="2"/>
@@ -1718,7 +1795,7 @@
       <c r="J17" s="2"/>
       <c r="K17" s="4"/>
     </row>
-    <row r="18" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:11" x14ac:dyDescent="0.35">
       <c r="B18" s="3"/>
       <c r="C18" s="16"/>
       <c r="D18" s="2"/>
@@ -1730,7 +1807,7 @@
       <c r="J18" s="2"/>
       <c r="K18" s="4"/>
     </row>
-    <row r="19" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:11" x14ac:dyDescent="0.35">
       <c r="B19" s="3"/>
       <c r="C19" s="16"/>
       <c r="D19" s="2"/>
@@ -1742,7 +1819,7 @@
       <c r="J19" s="2"/>
       <c r="K19" s="4"/>
     </row>
-    <row r="20" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:11" x14ac:dyDescent="0.35">
       <c r="B20" s="3"/>
       <c r="C20" s="16"/>
       <c r="D20" s="2"/>
@@ -1754,7 +1831,7 @@
       <c r="J20" s="2"/>
       <c r="K20" s="4"/>
     </row>
-    <row r="21" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:11" x14ac:dyDescent="0.35">
       <c r="B21" s="3"/>
       <c r="C21" s="16"/>
       <c r="D21" s="2"/>
@@ -1766,7 +1843,7 @@
       <c r="J21" s="2"/>
       <c r="K21" s="4"/>
     </row>
-    <row r="22" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:11" x14ac:dyDescent="0.35">
       <c r="B22" s="3"/>
       <c r="C22" s="16"/>
       <c r="D22" s="2"/>
@@ -1778,7 +1855,7 @@
       <c r="J22" s="2"/>
       <c r="K22" s="4"/>
     </row>
-    <row r="23" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:11" x14ac:dyDescent="0.35">
       <c r="B23" s="3"/>
       <c r="C23" s="16"/>
       <c r="D23" s="2"/>
@@ -1790,7 +1867,7 @@
       <c r="J23" s="2"/>
       <c r="K23" s="4"/>
     </row>
-    <row r="24" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:11" x14ac:dyDescent="0.35">
       <c r="B24" s="3"/>
       <c r="C24" s="16"/>
       <c r="D24" s="2"/>
@@ -1802,7 +1879,7 @@
       <c r="J24" s="2"/>
       <c r="K24" s="4"/>
     </row>
-    <row r="25" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:11" x14ac:dyDescent="0.35">
       <c r="B25" s="3"/>
       <c r="C25" s="16"/>
       <c r="D25" s="2"/>
@@ -1814,7 +1891,7 @@
       <c r="J25" s="2"/>
       <c r="K25" s="4"/>
     </row>
-    <row r="26" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="2:11" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B26" s="5"/>
       <c r="C26" s="17"/>
       <c r="D26" s="6"/>
@@ -1832,28 +1909,28 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="B1:K26"/>
   <sheetViews>
     <sheetView topLeftCell="B1" workbookViewId="0">
       <selection activeCell="J25" sqref="J25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="21.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="19.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="36.42578125" customWidth="1"/>
-    <col min="5" max="5" width="13.5703125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="7.42578125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="31.28515625" customWidth="1"/>
-    <col min="8" max="8" width="12.7109375" customWidth="1"/>
-    <col min="9" max="9" width="13.5703125" customWidth="1"/>
-    <col min="10" max="10" width="22.7109375" customWidth="1"/>
+    <col min="2" max="2" width="21.1796875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19.26953125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="36.453125" customWidth="1"/>
+    <col min="5" max="5" width="13.54296875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="7.453125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="31.26953125" customWidth="1"/>
+    <col min="8" max="8" width="12.7265625" customWidth="1"/>
+    <col min="9" max="9" width="13.54296875" customWidth="1"/>
+    <col min="10" max="10" width="22.7265625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="2" spans="2:11" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="2:11" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
+    <row r="2" spans="2:11" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B2" s="11" t="s">
         <v>13</v>
       </c>
@@ -1885,7 +1962,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:11" x14ac:dyDescent="0.35">
       <c r="B3" s="8" t="s">
         <v>9</v>
       </c>
@@ -1915,7 +1992,7 @@
       </c>
       <c r="K3" s="10"/>
     </row>
-    <row r="4" spans="2:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B4" s="8" t="s">
         <v>9</v>
       </c>
@@ -1945,7 +2022,7 @@
       </c>
       <c r="K4" s="4"/>
     </row>
-    <row r="5" spans="2:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:11" x14ac:dyDescent="0.35">
       <c r="B5" s="8" t="s">
         <v>9</v>
       </c>
@@ -1975,7 +2052,7 @@
       </c>
       <c r="K5" s="4"/>
     </row>
-    <row r="6" spans="2:11" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:11" ht="27.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B6" s="8" t="s">
         <v>9</v>
       </c>
@@ -2005,7 +2082,7 @@
       </c>
       <c r="K6" s="4"/>
     </row>
-    <row r="7" spans="2:11" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:11" ht="32.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B7" s="8" t="s">
         <v>9</v>
       </c>
@@ -2035,7 +2112,7 @@
       </c>
       <c r="K7" s="4"/>
     </row>
-    <row r="8" spans="2:11" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:11" ht="33" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B8" s="8" t="s">
         <v>9</v>
       </c>
@@ -2065,7 +2142,7 @@
       </c>
       <c r="K8" s="4"/>
     </row>
-    <row r="9" spans="2:11" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:11" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B9" s="8" t="s">
         <v>9</v>
       </c>
@@ -2095,7 +2172,7 @@
       </c>
       <c r="K9" s="4"/>
     </row>
-    <row r="10" spans="2:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:11" ht="29" x14ac:dyDescent="0.35">
       <c r="B10" s="8" t="s">
         <v>9</v>
       </c>
@@ -2125,7 +2202,7 @@
       </c>
       <c r="K10" s="4"/>
     </row>
-    <row r="11" spans="2:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:11" ht="29" x14ac:dyDescent="0.35">
       <c r="B11" s="8" t="s">
         <v>9</v>
       </c>
@@ -2155,7 +2232,7 @@
       </c>
       <c r="K11" s="4"/>
     </row>
-    <row r="12" spans="2:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:11" ht="29" x14ac:dyDescent="0.35">
       <c r="B12" s="8" t="s">
         <v>9</v>
       </c>
@@ -2185,7 +2262,7 @@
       </c>
       <c r="K12" s="4"/>
     </row>
-    <row r="13" spans="2:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:11" ht="29" x14ac:dyDescent="0.35">
       <c r="B13" s="8" t="s">
         <v>9</v>
       </c>
@@ -2215,7 +2292,7 @@
       </c>
       <c r="K13" s="4"/>
     </row>
-    <row r="14" spans="2:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:11" ht="29" x14ac:dyDescent="0.35">
       <c r="B14" s="8" t="s">
         <v>9</v>
       </c>
@@ -2245,7 +2322,7 @@
       </c>
       <c r="K14" s="4"/>
     </row>
-    <row r="15" spans="2:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:11" ht="29" x14ac:dyDescent="0.35">
       <c r="B15" s="8" t="s">
         <v>9</v>
       </c>
@@ -2275,7 +2352,7 @@
       </c>
       <c r="K15" s="4"/>
     </row>
-    <row r="16" spans="2:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:11" ht="29" x14ac:dyDescent="0.35">
       <c r="B16" s="8" t="s">
         <v>9</v>
       </c>
@@ -2305,7 +2382,7 @@
       </c>
       <c r="K16" s="4"/>
     </row>
-    <row r="17" spans="2:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:11" ht="29" x14ac:dyDescent="0.35">
       <c r="B17" s="8" t="s">
         <v>9</v>
       </c>
@@ -2335,7 +2412,7 @@
       </c>
       <c r="K17" s="4"/>
     </row>
-    <row r="18" spans="2:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:11" ht="29" x14ac:dyDescent="0.35">
       <c r="B18" s="8" t="s">
         <v>9</v>
       </c>
@@ -2365,7 +2442,7 @@
       </c>
       <c r="K18" s="4"/>
     </row>
-    <row r="19" spans="2:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:11" ht="29" x14ac:dyDescent="0.35">
       <c r="B19" s="8" t="s">
         <v>9</v>
       </c>
@@ -2395,7 +2472,7 @@
       </c>
       <c r="K19" s="4"/>
     </row>
-    <row r="20" spans="2:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:11" ht="29" x14ac:dyDescent="0.35">
       <c r="B20" s="8" t="s">
         <v>9</v>
       </c>
@@ -2425,7 +2502,7 @@
       </c>
       <c r="K20" s="4"/>
     </row>
-    <row r="21" spans="2:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:11" ht="29" x14ac:dyDescent="0.35">
       <c r="B21" s="8" t="s">
         <v>9</v>
       </c>
@@ -2455,7 +2532,7 @@
       </c>
       <c r="K21" s="4"/>
     </row>
-    <row r="22" spans="2:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:11" ht="29" x14ac:dyDescent="0.35">
       <c r="B22" s="8" t="s">
         <v>9</v>
       </c>
@@ -2485,7 +2562,7 @@
       </c>
       <c r="K22" s="4"/>
     </row>
-    <row r="23" spans="2:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:11" ht="29" x14ac:dyDescent="0.35">
       <c r="B23" s="8" t="s">
         <v>9</v>
       </c>
@@ -2515,7 +2592,7 @@
       </c>
       <c r="K23" s="4"/>
     </row>
-    <row r="24" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:11" x14ac:dyDescent="0.35">
       <c r="B24" s="8" t="s">
         <v>9</v>
       </c>
@@ -2545,7 +2622,7 @@
       </c>
       <c r="K24" s="4"/>
     </row>
-    <row r="25" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:11" x14ac:dyDescent="0.35">
       <c r="B25" s="8"/>
       <c r="C25" s="15"/>
       <c r="D25" s="18"/>
@@ -2557,7 +2634,7 @@
       <c r="J25" s="9"/>
       <c r="K25" s="4"/>
     </row>
-    <row r="26" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="2:11" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B26" s="8"/>
       <c r="C26" s="15"/>
       <c r="D26" s="18"/>
@@ -2575,63 +2652,63 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="H30" sqref="H30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J8"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
+  <dimension ref="A1:J11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I6" sqref="I6"/>
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="18.7109375" customWidth="1"/>
-    <col min="2" max="2" width="21.7109375" customWidth="1"/>
-    <col min="3" max="3" width="35.5703125" customWidth="1"/>
-    <col min="4" max="4" width="18.140625" customWidth="1"/>
-    <col min="5" max="5" width="17.42578125" customWidth="1"/>
-    <col min="6" max="6" width="33.140625" customWidth="1"/>
-    <col min="7" max="8" width="14.28515625" customWidth="1"/>
+    <col min="1" max="1" width="18.7265625" customWidth="1"/>
+    <col min="2" max="2" width="21.7265625" customWidth="1"/>
+    <col min="3" max="3" width="35.54296875" customWidth="1"/>
+    <col min="4" max="4" width="18.1796875" customWidth="1"/>
+    <col min="5" max="5" width="17.453125" customWidth="1"/>
+    <col min="6" max="6" width="33.1796875" customWidth="1"/>
+    <col min="7" max="8" width="14.26953125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="75.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:10" ht="73" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A1" s="11" t="s">
         <v>13</v>
       </c>
@@ -2663,7 +2740,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A2" s="8" t="s">
         <v>9</v>
       </c>
@@ -2693,7 +2770,7 @@
       </c>
       <c r="J2" s="10"/>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A3" s="8" t="s">
         <v>9</v>
       </c>
@@ -2723,7 +2800,7 @@
       </c>
       <c r="J3" s="4"/>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A4" s="8" t="s">
         <v>9</v>
       </c>
@@ -2753,7 +2830,7 @@
       </c>
       <c r="J4" s="4"/>
     </row>
-    <row r="5" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A5" s="8" t="s">
         <v>9</v>
       </c>
@@ -2783,7 +2860,7 @@
       </c>
       <c r="J5" s="4"/>
     </row>
-    <row r="6" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A6" s="8" t="s">
         <v>9</v>
       </c>
@@ -2813,29 +2890,152 @@
       </c>
       <c r="J6" s="4"/>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A7" s="8"/>
-      <c r="B7" s="15"/>
-      <c r="C7" s="18"/>
-      <c r="D7" s="9"/>
-      <c r="E7" s="9"/>
-      <c r="F7" s="9"/>
-      <c r="G7" s="19"/>
-      <c r="H7" s="9"/>
-      <c r="I7" s="9"/>
+    <row r="7" spans="1:10" ht="58" x14ac:dyDescent="0.35">
+      <c r="A7" s="20" t="s">
+        <v>9</v>
+      </c>
+      <c r="B7" s="21" t="s">
+        <v>79</v>
+      </c>
+      <c r="C7" s="22" t="s">
+        <v>54</v>
+      </c>
+      <c r="D7" s="23" t="s">
+        <v>10</v>
+      </c>
+      <c r="E7" s="23" t="s">
+        <v>10</v>
+      </c>
+      <c r="F7" s="18" t="s">
+        <v>82</v>
+      </c>
+      <c r="G7" s="24">
+        <v>44504</v>
+      </c>
+      <c r="H7" s="23" t="s">
+        <v>80</v>
+      </c>
+      <c r="I7" s="23" t="s">
+        <v>81</v>
+      </c>
       <c r="J7" s="4"/>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A8" s="8"/>
-      <c r="B8" s="15"/>
-      <c r="C8" s="18"/>
-      <c r="D8" s="9"/>
-      <c r="E8" s="9"/>
-      <c r="F8" s="18"/>
-      <c r="G8" s="19"/>
-      <c r="H8" s="9"/>
-      <c r="I8" s="9"/>
+    <row r="8" spans="1:10" ht="87" x14ac:dyDescent="0.35">
+      <c r="A8" s="20" t="s">
+        <v>9</v>
+      </c>
+      <c r="B8" s="21" t="s">
+        <v>83</v>
+      </c>
+      <c r="C8" s="22" t="s">
+        <v>46</v>
+      </c>
+      <c r="D8" s="23" t="s">
+        <v>10</v>
+      </c>
+      <c r="E8" s="23" t="s">
+        <v>10</v>
+      </c>
+      <c r="F8" s="18" t="s">
+        <v>84</v>
+      </c>
+      <c r="G8" s="24">
+        <v>44504</v>
+      </c>
+      <c r="H8" s="23" t="s">
+        <v>80</v>
+      </c>
+      <c r="I8" s="23" t="s">
+        <v>81</v>
+      </c>
       <c r="J8" s="4"/>
+    </row>
+    <row r="9" spans="1:10" ht="58" x14ac:dyDescent="0.35">
+      <c r="A9" s="25" t="s">
+        <v>9</v>
+      </c>
+      <c r="B9" s="26" t="s">
+        <v>85</v>
+      </c>
+      <c r="C9" s="26" t="s">
+        <v>48</v>
+      </c>
+      <c r="D9" s="27" t="s">
+        <v>10</v>
+      </c>
+      <c r="E9" s="27" t="s">
+        <v>10</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="G9" s="28">
+        <v>44504</v>
+      </c>
+      <c r="H9" s="27" t="s">
+        <v>80</v>
+      </c>
+      <c r="I9" s="27" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" ht="29" x14ac:dyDescent="0.35">
+      <c r="A10" s="25" t="s">
+        <v>9</v>
+      </c>
+      <c r="B10" s="26" t="s">
+        <v>87</v>
+      </c>
+      <c r="C10" s="26" t="s">
+        <v>50</v>
+      </c>
+      <c r="D10" s="27" t="s">
+        <v>10</v>
+      </c>
+      <c r="E10" s="27" t="s">
+        <v>10</v>
+      </c>
+      <c r="F10" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="G10" s="28">
+        <v>44504</v>
+      </c>
+      <c r="H10" s="27" t="s">
+        <v>80</v>
+      </c>
+      <c r="I10" s="27" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A11" s="25" t="s">
+        <v>9</v>
+      </c>
+      <c r="B11" s="26" t="s">
+        <v>89</v>
+      </c>
+      <c r="C11" s="26" t="s">
+        <v>52</v>
+      </c>
+      <c r="D11" s="27" t="s">
+        <v>10</v>
+      </c>
+      <c r="E11" s="27" t="s">
+        <v>10</v>
+      </c>
+      <c r="F11" t="s">
+        <v>90</v>
+      </c>
+      <c r="G11" s="28">
+        <v>44504</v>
+      </c>
+      <c r="H11" s="27" t="s">
+        <v>80</v>
+      </c>
+      <c r="I11" s="27" t="s">
+        <v>81</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
class architecte and condotierre and cahierDeTests edit
</commit_message>
<xml_diff>
--- a/src/ressources/cahierDeTests.xlsx
+++ b/src/ressources/cahierDeTests.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\askri\git\Citadelle\src\ressources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C4B23CAA-6033-4324-938F-81B1207B7265}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{10B3A935-E39B-45A4-BE5D-B8FC77BACA4D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" firstSheet="3" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="396" uniqueCount="91">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="412" uniqueCount="96">
   <si>
     <t>Objectif</t>
   </si>
@@ -315,6 +315,21 @@
   </si>
   <si>
     <t>test de la réinitialisation</t>
+  </si>
+  <si>
+    <t xml:space="preserve">		test.test1();</t>
+  </si>
+  <si>
+    <t>test du nom du personnage, test du rang du personnage, test des caractéristiques du personnage, test de l'initialisation de la variable "joueur", test de l'initialisation de la variable "assassine", test de l'initialisation de la variable "vole".</t>
+  </si>
+  <si>
+    <t xml:space="preserve">		test.test2();	</t>
+  </si>
+  <si>
+    <t>TEST DE L'UTILISATION DU POUVOIR</t>
+  </si>
+  <si>
+    <t>test du nombre de cartes dans la main avant l'utilisation du pouvoir, vous avez pioché 2 cartes quartier supplémentaires !, test du nombre de cartes dans la main après l'utilisation du pouvoir.</t>
   </si>
 </sst>
 </file>
@@ -589,7 +604,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -645,6 +660,13 @@
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2691,10 +2713,10 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
-  <dimension ref="A1:J11"/>
+  <dimension ref="A1:J13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="L13" sqref="L13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -3037,6 +3059,64 @@
         <v>81</v>
       </c>
     </row>
+    <row r="12" spans="1:10" ht="101.5" x14ac:dyDescent="0.35">
+      <c r="A12" s="25" t="s">
+        <v>9</v>
+      </c>
+      <c r="B12" s="29" t="s">
+        <v>91</v>
+      </c>
+      <c r="C12" s="26" t="s">
+        <v>54</v>
+      </c>
+      <c r="D12" s="27" t="s">
+        <v>10</v>
+      </c>
+      <c r="E12" s="27" t="s">
+        <v>10</v>
+      </c>
+      <c r="F12" s="30" t="s">
+        <v>92</v>
+      </c>
+      <c r="G12" s="31">
+        <v>44557</v>
+      </c>
+      <c r="H12" s="27" t="s">
+        <v>80</v>
+      </c>
+      <c r="I12" s="27" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A13" s="25" t="s">
+        <v>9</v>
+      </c>
+      <c r="B13" s="29" t="s">
+        <v>93</v>
+      </c>
+      <c r="C13" t="s">
+        <v>94</v>
+      </c>
+      <c r="D13" s="27" t="s">
+        <v>10</v>
+      </c>
+      <c r="E13" s="27" t="s">
+        <v>10</v>
+      </c>
+      <c r="F13" t="s">
+        <v>95</v>
+      </c>
+      <c r="G13" s="31">
+        <v>44557</v>
+      </c>
+      <c r="H13" s="27" t="s">
+        <v>80</v>
+      </c>
+      <c r="I13" s="27" t="s">
+        <v>81</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
remplir le cahier de charge
</commit_message>
<xml_diff>
--- a/src/ressources/cahierDeTests.xlsx
+++ b/src/ressources/cahierDeTests.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24701"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\askri\git\Citadelle\src\ressources\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\USER\eclipse-workspace\Citadelle\src\ressources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{10B3A935-E39B-45A4-BE5D-B8FC77BACA4D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" firstSheet="3" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-105" yWindow="-105" windowWidth="19425" windowHeight="10425" firstSheet="6" activeTab="10"/>
   </bookViews>
   <sheets>
     <sheet name="Objectifs" sheetId="1" r:id="rId1"/>
@@ -19,8 +18,11 @@
     <sheet name="test.TestRoi" sheetId="4" r:id="rId4"/>
     <sheet name="test.TestPioche" sheetId="5" r:id="rId5"/>
     <sheet name="test.TestPlateauDeJeu" sheetId="6" r:id="rId6"/>
-    <sheet name="test..." sheetId="7" r:id="rId7"/>
-    <sheet name="test.TestMagicienne" sheetId="8" r:id="rId8"/>
+    <sheet name="test.TestAssassin" sheetId="7" r:id="rId7"/>
+    <sheet name="test.TestVoleur" sheetId="9" r:id="rId8"/>
+    <sheet name="test.TestMagicienne" sheetId="8" r:id="rId9"/>
+    <sheet name="test.TestEveque" sheetId="10" r:id="rId10"/>
+    <sheet name="test.TestMarchande" sheetId="11" r:id="rId11"/>
   </sheets>
   <calcPr calcId="0"/>
   <extLst>
@@ -32,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="412" uniqueCount="96">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="632" uniqueCount="138">
   <si>
     <t>Objectif</t>
   </si>
@@ -330,12 +332,138 @@
   </si>
   <si>
     <t>test du nombre de cartes dans la main avant l'utilisation du pouvoir, vous avez pioché 2 cartes quartier supplémentaires !, test du nombre de cartes dans la main après l'utilisation du pouvoir.</t>
+  </si>
+  <si>
+    <t>TestPioche.test1()</t>
+  </si>
+  <si>
+    <t>TestPioche.test2()</t>
+  </si>
+  <si>
+    <t>TestPioche.test3()</t>
+  </si>
+  <si>
+    <t>TestPioche.test4()</t>
+  </si>
+  <si>
+    <t>TEST DE L'AJOUT D'UN QUARTIER</t>
+  </si>
+  <si>
+    <t>TEST DU RETRAIT D'UN QUARTIER</t>
+  </si>
+  <si>
+    <t>TEST DU MELANGE DE LA PIOCHE</t>
+  </si>
+  <si>
+    <t>Badugue Igor</t>
+  </si>
+  <si>
+    <t>un quartier est bien ajouté</t>
+  </si>
+  <si>
+    <t>un quartier est bien retirer</t>
+  </si>
+  <si>
+    <t>le melange est bien effectuer sans erreurs</t>
+  </si>
+  <si>
+    <t>TestPlateauDeJeu.test1()</t>
+  </si>
+  <si>
+    <t>TestPlateauDeJeu.test2()</t>
+  </si>
+  <si>
+    <t>TestPlateauDeJeu.test3()</t>
+  </si>
+  <si>
+    <t>TestPlateauDeJeu.test4()</t>
+  </si>
+  <si>
+    <t>TEST DE L'AJOUT D'UN JOUEUR</t>
+  </si>
+  <si>
+    <t>TEST DE L'AJOUT D'UN PERSONNAGE</t>
+  </si>
+  <si>
+    <t>TEST DE L'ASSOCIATION DU PLATEAU AU PERSONNAGE</t>
+  </si>
+  <si>
+    <t>un joueur est bien ajouté</t>
+  </si>
+  <si>
+    <t>un personnage est bien retirer</t>
+  </si>
+  <si>
+    <t>pour chaque personnage créer il est bien associé au plateau</t>
+  </si>
+  <si>
+    <t>TestAssassin.test1()</t>
+  </si>
+  <si>
+    <t>TestAssassin.test2()</t>
+  </si>
+  <si>
+    <t>type de test+A1:J6 (unitaire, intégration, validation)</t>
+  </si>
+  <si>
+    <t>TEST DE L'ASSASSINAT DU ROI</t>
+  </si>
+  <si>
+    <t>elimination du roi</t>
+  </si>
+  <si>
+    <t>le roi est bien assassiné</t>
+  </si>
+  <si>
+    <t>TestVoleur.test1()</t>
+  </si>
+  <si>
+    <t>TestVoleur.test2()</t>
+  </si>
+  <si>
+    <t>TEST DU VOL DU ROI</t>
+  </si>
+  <si>
+    <t>le roi est bien volé</t>
+  </si>
+  <si>
+    <t>type de test(unitaire, intégration, validation)</t>
+  </si>
+  <si>
+    <t>TestEveque.test1()</t>
+  </si>
+  <si>
+    <t>TestEveque.test2()</t>
+  </si>
+  <si>
+    <t>test du nombre de pieces d'or avant et apres percepetion des ressources</t>
+  </si>
+  <si>
+    <t>Batcho Loan</t>
+  </si>
+  <si>
+    <t>test le constructeur et les caracteristiques de l'eveque</t>
+  </si>
+  <si>
+    <t>TEST DE LA PERCEPTION DE RESSOURCES SPECIFIQUES ET DE L'UTILISATEUR DU POUVOIR</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TEST DU CONSTRUCTEUR </t>
+  </si>
+  <si>
+    <t>test du nombre de pieces d'or avant et apres percepetion des ressources, test aussi le nombre de pieces d'or apres utilisation des pouvoirs</t>
+  </si>
+  <si>
+    <t>TestMarchande.test1()</t>
+  </si>
+  <si>
+    <t>TestMarchande.test2()</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -359,7 +487,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="18">
+  <borders count="31">
     <border>
       <left/>
       <right/>
@@ -600,11 +728,180 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="53">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -667,6 +964,35 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="23" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="29" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -980,37 +1306,327 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:B5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="77.26953125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="77.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:2" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="2" spans="2:2" ht="45" x14ac:dyDescent="0.25">
       <c r="B2" s="1" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="3" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="3" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="4" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="4" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="5" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="5" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
         <v>31</v>
       </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:J4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:J4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="23" customWidth="1"/>
+    <col min="2" max="2" width="22.7109375" customWidth="1"/>
+    <col min="3" max="3" width="24.140625" customWidth="1"/>
+    <col min="6" max="6" width="41.7109375" customWidth="1"/>
+    <col min="9" max="9" width="19.5703125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" ht="48" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="42" t="s">
+        <v>127</v>
+      </c>
+      <c r="B1" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="C1" s="12" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1" s="12" t="s">
+        <v>1</v>
+      </c>
+      <c r="E1" s="12" t="s">
+        <v>2</v>
+      </c>
+      <c r="F1" s="12" t="s">
+        <v>3</v>
+      </c>
+      <c r="G1" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="H1" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="I1" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="J1" s="14" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="A2" s="43" t="s">
+        <v>9</v>
+      </c>
+      <c r="B2" s="8" t="s">
+        <v>128</v>
+      </c>
+      <c r="C2" s="9" t="s">
+        <v>54</v>
+      </c>
+      <c r="D2" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="E2" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="F2" s="18" t="s">
+        <v>132</v>
+      </c>
+      <c r="G2" s="19">
+        <v>44554</v>
+      </c>
+      <c r="H2" s="9" t="s">
+        <v>131</v>
+      </c>
+      <c r="I2" s="9" t="s">
+        <v>39</v>
+      </c>
+      <c r="J2" s="10"/>
+    </row>
+    <row r="3" spans="1:10" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="43" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3" s="8" t="s">
+        <v>129</v>
+      </c>
+      <c r="C3" s="18" t="s">
+        <v>67</v>
+      </c>
+      <c r="D3" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="E3" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="F3" s="18" t="s">
+        <v>130</v>
+      </c>
+      <c r="G3" s="19">
+        <v>44555</v>
+      </c>
+      <c r="H3" s="9" t="s">
+        <v>131</v>
+      </c>
+      <c r="I3" s="9" t="s">
+        <v>61</v>
+      </c>
+      <c r="J3" s="4"/>
+    </row>
+    <row r="4" spans="1:10" ht="45" x14ac:dyDescent="0.25">
+      <c r="A4" s="43" t="s">
+        <v>9</v>
+      </c>
+      <c r="B4" s="8" t="s">
+        <v>129</v>
+      </c>
+      <c r="C4" s="18" t="s">
+        <v>67</v>
+      </c>
+      <c r="D4" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="E4" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="F4" s="18" t="s">
+        <v>130</v>
+      </c>
+      <c r="G4" s="19">
+        <v>44556</v>
+      </c>
+      <c r="H4" s="9" t="s">
+        <v>131</v>
+      </c>
+      <c r="I4" s="9" t="s">
+        <v>39</v>
+      </c>
+      <c r="J4" s="4"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:J4"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="23.5703125" customWidth="1"/>
+    <col min="2" max="2" width="23" customWidth="1"/>
+    <col min="3" max="3" width="24.140625" customWidth="1"/>
+    <col min="4" max="4" width="15.7109375" customWidth="1"/>
+    <col min="6" max="6" width="20.85546875" customWidth="1"/>
+    <col min="7" max="7" width="12.140625" customWidth="1"/>
+    <col min="8" max="8" width="11.85546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" ht="40.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="42" t="s">
+        <v>127</v>
+      </c>
+      <c r="B1" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="C1" s="12" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1" s="12" t="s">
+        <v>1</v>
+      </c>
+      <c r="E1" s="12" t="s">
+        <v>2</v>
+      </c>
+      <c r="F1" s="12" t="s">
+        <v>3</v>
+      </c>
+      <c r="G1" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="H1" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="I1" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="J1" s="14" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" ht="49.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="47" t="s">
+        <v>9</v>
+      </c>
+      <c r="B2" s="48" t="s">
+        <v>136</v>
+      </c>
+      <c r="C2" s="49" t="s">
+        <v>134</v>
+      </c>
+      <c r="D2" s="49" t="s">
+        <v>10</v>
+      </c>
+      <c r="E2" s="49" t="s">
+        <v>10</v>
+      </c>
+      <c r="F2" s="50" t="s">
+        <v>132</v>
+      </c>
+      <c r="G2" s="51">
+        <v>44559</v>
+      </c>
+      <c r="H2" s="49" t="s">
+        <v>131</v>
+      </c>
+      <c r="I2" s="49" t="s">
+        <v>39</v>
+      </c>
+      <c r="J2" s="52"/>
+    </row>
+    <row r="3" spans="1:10" ht="105" x14ac:dyDescent="0.25">
+      <c r="A3" s="43" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3" s="8" t="s">
+        <v>137</v>
+      </c>
+      <c r="C3" s="18" t="s">
+        <v>133</v>
+      </c>
+      <c r="D3" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="E3" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="F3" s="18" t="s">
+        <v>135</v>
+      </c>
+      <c r="G3" s="19">
+        <v>44560</v>
+      </c>
+      <c r="H3" s="9" t="s">
+        <v>131</v>
+      </c>
+      <c r="I3" s="9" t="s">
+        <v>61</v>
+      </c>
+      <c r="J3" s="4"/>
+    </row>
+    <row r="4" spans="1:10" ht="105.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="44" t="s">
+        <v>9</v>
+      </c>
+      <c r="B4" s="32" t="s">
+        <v>137</v>
+      </c>
+      <c r="C4" s="34" t="s">
+        <v>133</v>
+      </c>
+      <c r="D4" s="35" t="s">
+        <v>10</v>
+      </c>
+      <c r="E4" s="35" t="s">
+        <v>10</v>
+      </c>
+      <c r="F4" s="34" t="s">
+        <v>135</v>
+      </c>
+      <c r="G4" s="36">
+        <v>44561</v>
+      </c>
+      <c r="H4" s="35" t="s">
+        <v>131</v>
+      </c>
+      <c r="I4" s="35" t="s">
+        <v>39</v>
+      </c>
+      <c r="J4" s="7"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1018,30 +1634,30 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:K26"/>
   <sheetViews>
-    <sheetView topLeftCell="D2" workbookViewId="0">
-      <selection activeCell="B3" sqref="B2:K9"/>
+    <sheetView topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2:J9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="3.54296875" customWidth="1"/>
-    <col min="2" max="2" width="20.7265625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="18.1796875" customWidth="1"/>
-    <col min="4" max="4" width="27.7265625" customWidth="1"/>
-    <col min="5" max="5" width="12.7265625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="8.81640625" customWidth="1"/>
+    <col min="1" max="1" width="3.5703125" customWidth="1"/>
+    <col min="2" max="2" width="20.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.140625" customWidth="1"/>
+    <col min="4" max="4" width="27.7109375" customWidth="1"/>
+    <col min="5" max="5" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="8.85546875" customWidth="1"/>
     <col min="7" max="7" width="31" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="11.7265625" customWidth="1"/>
-    <col min="9" max="9" width="9.1796875" customWidth="1"/>
-    <col min="10" max="10" width="21.453125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="48.1796875" customWidth="1"/>
+    <col min="8" max="8" width="11.7109375" customWidth="1"/>
+    <col min="9" max="9" width="9.140625" customWidth="1"/>
+    <col min="10" max="10" width="21.42578125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="48.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:11" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
-    <row r="2" spans="2:11" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="2" spans="2:11" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B2" s="11" t="s">
         <v>13</v>
       </c>
@@ -1073,7 +1689,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="2:11" x14ac:dyDescent="0.35">
+    <row r="3" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B3" s="8" t="s">
         <v>9</v>
       </c>
@@ -1103,7 +1719,7 @@
       </c>
       <c r="K3" s="10"/>
     </row>
-    <row r="4" spans="2:11" ht="29" x14ac:dyDescent="0.35">
+    <row r="4" spans="2:11" ht="30" x14ac:dyDescent="0.25">
       <c r="B4" s="8" t="s">
         <v>9</v>
       </c>
@@ -1133,7 +1749,7 @@
       </c>
       <c r="K4" s="4"/>
     </row>
-    <row r="5" spans="2:11" ht="29" x14ac:dyDescent="0.35">
+    <row r="5" spans="2:11" ht="30" x14ac:dyDescent="0.25">
       <c r="B5" s="8" t="s">
         <v>9</v>
       </c>
@@ -1163,7 +1779,7 @@
       </c>
       <c r="K5" s="4"/>
     </row>
-    <row r="6" spans="2:11" ht="29" x14ac:dyDescent="0.35">
+    <row r="6" spans="2:11" ht="30" x14ac:dyDescent="0.25">
       <c r="B6" s="8" t="s">
         <v>9</v>
       </c>
@@ -1193,7 +1809,7 @@
       </c>
       <c r="K6" s="4"/>
     </row>
-    <row r="7" spans="2:11" ht="29" x14ac:dyDescent="0.35">
+    <row r="7" spans="2:11" ht="30" x14ac:dyDescent="0.25">
       <c r="B7" s="8" t="s">
         <v>9</v>
       </c>
@@ -1223,7 +1839,7 @@
       </c>
       <c r="K7" s="4"/>
     </row>
-    <row r="8" spans="2:11" ht="29" x14ac:dyDescent="0.35">
+    <row r="8" spans="2:11" ht="30" x14ac:dyDescent="0.25">
       <c r="B8" s="8" t="s">
         <v>9</v>
       </c>
@@ -1253,7 +1869,7 @@
       </c>
       <c r="K8" s="4"/>
     </row>
-    <row r="9" spans="2:11" ht="29" x14ac:dyDescent="0.35">
+    <row r="9" spans="2:11" ht="30" x14ac:dyDescent="0.25">
       <c r="B9" s="8" t="s">
         <v>9</v>
       </c>
@@ -1283,7 +1899,7 @@
       </c>
       <c r="K9" s="4"/>
     </row>
-    <row r="10" spans="2:11" x14ac:dyDescent="0.35">
+    <row r="10" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B10" s="3"/>
       <c r="C10" s="16"/>
       <c r="D10" s="2"/>
@@ -1295,7 +1911,7 @@
       <c r="J10" s="2"/>
       <c r="K10" s="4"/>
     </row>
-    <row r="11" spans="2:11" x14ac:dyDescent="0.35">
+    <row r="11" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B11" s="3"/>
       <c r="C11" s="16"/>
       <c r="D11" s="2"/>
@@ -1307,7 +1923,7 @@
       <c r="J11" s="2"/>
       <c r="K11" s="4"/>
     </row>
-    <row r="12" spans="2:11" x14ac:dyDescent="0.35">
+    <row r="12" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B12" s="3"/>
       <c r="C12" s="16"/>
       <c r="D12" s="2"/>
@@ -1319,7 +1935,7 @@
       <c r="J12" s="2"/>
       <c r="K12" s="4"/>
     </row>
-    <row r="13" spans="2:11" x14ac:dyDescent="0.35">
+    <row r="13" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B13" s="3"/>
       <c r="C13" s="16"/>
       <c r="D13" s="2"/>
@@ -1331,7 +1947,7 @@
       <c r="J13" s="2"/>
       <c r="K13" s="4"/>
     </row>
-    <row r="14" spans="2:11" x14ac:dyDescent="0.35">
+    <row r="14" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B14" s="3"/>
       <c r="C14" s="16"/>
       <c r="D14" s="2"/>
@@ -1343,7 +1959,7 @@
       <c r="J14" s="2"/>
       <c r="K14" s="4"/>
     </row>
-    <row r="15" spans="2:11" x14ac:dyDescent="0.35">
+    <row r="15" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B15" s="3"/>
       <c r="C15" s="16"/>
       <c r="D15" s="2"/>
@@ -1355,7 +1971,7 @@
       <c r="J15" s="2"/>
       <c r="K15" s="4"/>
     </row>
-    <row r="16" spans="2:11" x14ac:dyDescent="0.35">
+    <row r="16" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B16" s="3"/>
       <c r="C16" s="16"/>
       <c r="D16" s="2"/>
@@ -1367,7 +1983,7 @@
       <c r="J16" s="2"/>
       <c r="K16" s="4"/>
     </row>
-    <row r="17" spans="2:11" x14ac:dyDescent="0.35">
+    <row r="17" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B17" s="3"/>
       <c r="C17" s="16"/>
       <c r="D17" s="2"/>
@@ -1379,7 +1995,7 @@
       <c r="J17" s="2"/>
       <c r="K17" s="4"/>
     </row>
-    <row r="18" spans="2:11" x14ac:dyDescent="0.35">
+    <row r="18" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B18" s="3"/>
       <c r="C18" s="16"/>
       <c r="D18" s="2"/>
@@ -1391,7 +2007,7 @@
       <c r="J18" s="2"/>
       <c r="K18" s="4"/>
     </row>
-    <row r="19" spans="2:11" x14ac:dyDescent="0.35">
+    <row r="19" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B19" s="3"/>
       <c r="C19" s="16"/>
       <c r="D19" s="2"/>
@@ -1403,7 +2019,7 @@
       <c r="J19" s="2"/>
       <c r="K19" s="4"/>
     </row>
-    <row r="20" spans="2:11" x14ac:dyDescent="0.35">
+    <row r="20" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B20" s="3"/>
       <c r="C20" s="16"/>
       <c r="D20" s="2"/>
@@ -1415,7 +2031,7 @@
       <c r="J20" s="2"/>
       <c r="K20" s="4"/>
     </row>
-    <row r="21" spans="2:11" x14ac:dyDescent="0.35">
+    <row r="21" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B21" s="3"/>
       <c r="C21" s="16"/>
       <c r="D21" s="2"/>
@@ -1427,7 +2043,7 @@
       <c r="J21" s="2"/>
       <c r="K21" s="4"/>
     </row>
-    <row r="22" spans="2:11" x14ac:dyDescent="0.35">
+    <row r="22" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B22" s="3"/>
       <c r="C22" s="16"/>
       <c r="D22" s="2"/>
@@ -1439,7 +2055,7 @@
       <c r="J22" s="2"/>
       <c r="K22" s="4"/>
     </row>
-    <row r="23" spans="2:11" x14ac:dyDescent="0.35">
+    <row r="23" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B23" s="3"/>
       <c r="C23" s="16"/>
       <c r="D23" s="2"/>
@@ -1451,7 +2067,7 @@
       <c r="J23" s="2"/>
       <c r="K23" s="4"/>
     </row>
-    <row r="24" spans="2:11" x14ac:dyDescent="0.35">
+    <row r="24" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B24" s="3"/>
       <c r="C24" s="16"/>
       <c r="D24" s="2"/>
@@ -1463,7 +2079,7 @@
       <c r="J24" s="2"/>
       <c r="K24" s="4"/>
     </row>
-    <row r="25" spans="2:11" x14ac:dyDescent="0.35">
+    <row r="25" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B25" s="3"/>
       <c r="C25" s="16"/>
       <c r="D25" s="2"/>
@@ -1475,7 +2091,7 @@
       <c r="J25" s="2"/>
       <c r="K25" s="4"/>
     </row>
-    <row r="26" spans="2:11" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="26" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B26" s="5"/>
       <c r="C26" s="17"/>
       <c r="D26" s="6"/>
@@ -1493,29 +2109,29 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:K26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="21.54296875" customWidth="1"/>
-    <col min="3" max="3" width="19.7265625" customWidth="1"/>
-    <col min="4" max="4" width="26.81640625" customWidth="1"/>
-    <col min="5" max="5" width="13.54296875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="7.453125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="21.5703125" customWidth="1"/>
+    <col min="3" max="3" width="19.7109375" customWidth="1"/>
+    <col min="4" max="4" width="26.85546875" customWidth="1"/>
+    <col min="5" max="5" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="7.42578125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="31" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="14.7265625" customWidth="1"/>
-    <col min="9" max="9" width="14.26953125" customWidth="1"/>
-    <col min="10" max="10" width="27.81640625" customWidth="1"/>
-    <col min="11" max="11" width="59.26953125" customWidth="1"/>
+    <col min="8" max="8" width="14.7109375" customWidth="1"/>
+    <col min="9" max="9" width="14.28515625" customWidth="1"/>
+    <col min="10" max="10" width="27.85546875" customWidth="1"/>
+    <col min="11" max="11" width="59.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:11" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
-    <row r="2" spans="2:11" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="2" spans="2:11" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B2" s="11" t="s">
         <v>13</v>
       </c>
@@ -1547,7 +2163,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="2:11" x14ac:dyDescent="0.35">
+    <row r="3" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B3" s="8" t="s">
         <v>9</v>
       </c>
@@ -1577,7 +2193,7 @@
       </c>
       <c r="K3" s="10"/>
     </row>
-    <row r="4" spans="2:11" x14ac:dyDescent="0.35">
+    <row r="4" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B4" s="8" t="s">
         <v>9</v>
       </c>
@@ -1607,7 +2223,7 @@
       </c>
       <c r="K4" s="4"/>
     </row>
-    <row r="5" spans="2:11" x14ac:dyDescent="0.35">
+    <row r="5" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B5" s="8" t="s">
         <v>9</v>
       </c>
@@ -1637,7 +2253,7 @@
       </c>
       <c r="K5" s="4"/>
     </row>
-    <row r="6" spans="2:11" x14ac:dyDescent="0.35">
+    <row r="6" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B6" s="8" t="s">
         <v>9</v>
       </c>
@@ -1667,7 +2283,7 @@
       </c>
       <c r="K6" s="4"/>
     </row>
-    <row r="7" spans="2:11" ht="29" x14ac:dyDescent="0.35">
+    <row r="7" spans="2:11" ht="30" x14ac:dyDescent="0.25">
       <c r="B7" s="8" t="s">
         <v>9</v>
       </c>
@@ -1697,7 +2313,7 @@
       </c>
       <c r="K7" s="4"/>
     </row>
-    <row r="8" spans="2:11" x14ac:dyDescent="0.35">
+    <row r="8" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B8" s="8"/>
       <c r="C8" s="15"/>
       <c r="D8" s="18"/>
@@ -1709,7 +2325,7 @@
       <c r="J8" s="2"/>
       <c r="K8" s="4"/>
     </row>
-    <row r="9" spans="2:11" x14ac:dyDescent="0.35">
+    <row r="9" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B9" s="8"/>
       <c r="C9" s="15"/>
       <c r="D9" s="18"/>
@@ -1721,7 +2337,7 @@
       <c r="J9" s="2"/>
       <c r="K9" s="4"/>
     </row>
-    <row r="10" spans="2:11" x14ac:dyDescent="0.35">
+    <row r="10" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B10" s="3"/>
       <c r="C10" s="16"/>
       <c r="D10" s="2"/>
@@ -1733,7 +2349,7 @@
       <c r="J10" s="2"/>
       <c r="K10" s="4"/>
     </row>
-    <row r="11" spans="2:11" x14ac:dyDescent="0.35">
+    <row r="11" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B11" s="3"/>
       <c r="C11" s="16"/>
       <c r="D11" s="2"/>
@@ -1745,7 +2361,7 @@
       <c r="J11" s="2"/>
       <c r="K11" s="4"/>
     </row>
-    <row r="12" spans="2:11" x14ac:dyDescent="0.35">
+    <row r="12" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B12" s="3"/>
       <c r="C12" s="16"/>
       <c r="D12" s="2"/>
@@ -1757,7 +2373,7 @@
       <c r="J12" s="2"/>
       <c r="K12" s="4"/>
     </row>
-    <row r="13" spans="2:11" x14ac:dyDescent="0.35">
+    <row r="13" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B13" s="3"/>
       <c r="C13" s="16"/>
       <c r="D13" s="2"/>
@@ -1769,7 +2385,7 @@
       <c r="J13" s="2"/>
       <c r="K13" s="4"/>
     </row>
-    <row r="14" spans="2:11" x14ac:dyDescent="0.35">
+    <row r="14" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B14" s="3"/>
       <c r="C14" s="16"/>
       <c r="D14" s="2"/>
@@ -1781,7 +2397,7 @@
       <c r="J14" s="2"/>
       <c r="K14" s="4"/>
     </row>
-    <row r="15" spans="2:11" x14ac:dyDescent="0.35">
+    <row r="15" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B15" s="3"/>
       <c r="C15" s="16"/>
       <c r="D15" s="2"/>
@@ -1793,7 +2409,7 @@
       <c r="J15" s="2"/>
       <c r="K15" s="4"/>
     </row>
-    <row r="16" spans="2:11" x14ac:dyDescent="0.35">
+    <row r="16" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B16" s="3"/>
       <c r="C16" s="16"/>
       <c r="D16" s="2"/>
@@ -1805,7 +2421,7 @@
       <c r="J16" s="2"/>
       <c r="K16" s="4"/>
     </row>
-    <row r="17" spans="2:11" x14ac:dyDescent="0.35">
+    <row r="17" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B17" s="3"/>
       <c r="C17" s="16"/>
       <c r="D17" s="2"/>
@@ -1817,7 +2433,7 @@
       <c r="J17" s="2"/>
       <c r="K17" s="4"/>
     </row>
-    <row r="18" spans="2:11" x14ac:dyDescent="0.35">
+    <row r="18" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B18" s="3"/>
       <c r="C18" s="16"/>
       <c r="D18" s="2"/>
@@ -1829,7 +2445,7 @@
       <c r="J18" s="2"/>
       <c r="K18" s="4"/>
     </row>
-    <row r="19" spans="2:11" x14ac:dyDescent="0.35">
+    <row r="19" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B19" s="3"/>
       <c r="C19" s="16"/>
       <c r="D19" s="2"/>
@@ -1841,7 +2457,7 @@
       <c r="J19" s="2"/>
       <c r="K19" s="4"/>
     </row>
-    <row r="20" spans="2:11" x14ac:dyDescent="0.35">
+    <row r="20" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B20" s="3"/>
       <c r="C20" s="16"/>
       <c r="D20" s="2"/>
@@ -1853,7 +2469,7 @@
       <c r="J20" s="2"/>
       <c r="K20" s="4"/>
     </row>
-    <row r="21" spans="2:11" x14ac:dyDescent="0.35">
+    <row r="21" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B21" s="3"/>
       <c r="C21" s="16"/>
       <c r="D21" s="2"/>
@@ -1865,7 +2481,7 @@
       <c r="J21" s="2"/>
       <c r="K21" s="4"/>
     </row>
-    <row r="22" spans="2:11" x14ac:dyDescent="0.35">
+    <row r="22" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B22" s="3"/>
       <c r="C22" s="16"/>
       <c r="D22" s="2"/>
@@ -1877,7 +2493,7 @@
       <c r="J22" s="2"/>
       <c r="K22" s="4"/>
     </row>
-    <row r="23" spans="2:11" x14ac:dyDescent="0.35">
+    <row r="23" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B23" s="3"/>
       <c r="C23" s="16"/>
       <c r="D23" s="2"/>
@@ -1889,7 +2505,7 @@
       <c r="J23" s="2"/>
       <c r="K23" s="4"/>
     </row>
-    <row r="24" spans="2:11" x14ac:dyDescent="0.35">
+    <row r="24" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B24" s="3"/>
       <c r="C24" s="16"/>
       <c r="D24" s="2"/>
@@ -1901,7 +2517,7 @@
       <c r="J24" s="2"/>
       <c r="K24" s="4"/>
     </row>
-    <row r="25" spans="2:11" x14ac:dyDescent="0.35">
+    <row r="25" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B25" s="3"/>
       <c r="C25" s="16"/>
       <c r="D25" s="2"/>
@@ -1913,7 +2529,7 @@
       <c r="J25" s="2"/>
       <c r="K25" s="4"/>
     </row>
-    <row r="26" spans="2:11" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="26" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B26" s="5"/>
       <c r="C26" s="17"/>
       <c r="D26" s="6"/>
@@ -1931,28 +2547,28 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:K26"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="J25" sqref="J25"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2:K26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="21.1796875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="19.26953125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="36.453125" customWidth="1"/>
-    <col min="5" max="5" width="13.54296875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="7.453125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="31.26953125" customWidth="1"/>
-    <col min="8" max="8" width="12.7265625" customWidth="1"/>
-    <col min="9" max="9" width="13.54296875" customWidth="1"/>
-    <col min="10" max="10" width="22.7265625" customWidth="1"/>
+    <col min="2" max="2" width="21.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="36.42578125" customWidth="1"/>
+    <col min="5" max="5" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="7.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="31.28515625" customWidth="1"/>
+    <col min="8" max="8" width="12.7109375" customWidth="1"/>
+    <col min="9" max="9" width="13.5703125" customWidth="1"/>
+    <col min="10" max="10" width="22.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:11" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
-    <row r="2" spans="2:11" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="2" spans="2:11" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B2" s="11" t="s">
         <v>13</v>
       </c>
@@ -1984,7 +2600,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="2:11" x14ac:dyDescent="0.35">
+    <row r="3" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B3" s="8" t="s">
         <v>9</v>
       </c>
@@ -2014,7 +2630,7 @@
       </c>
       <c r="K3" s="10"/>
     </row>
-    <row r="4" spans="2:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="2:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B4" s="8" t="s">
         <v>9</v>
       </c>
@@ -2044,7 +2660,7 @@
       </c>
       <c r="K4" s="4"/>
     </row>
-    <row r="5" spans="2:11" x14ac:dyDescent="0.35">
+    <row r="5" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B5" s="8" t="s">
         <v>9</v>
       </c>
@@ -2074,7 +2690,7 @@
       </c>
       <c r="K5" s="4"/>
     </row>
-    <row r="6" spans="2:11" ht="27.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="2:11" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B6" s="8" t="s">
         <v>9</v>
       </c>
@@ -2104,7 +2720,7 @@
       </c>
       <c r="K6" s="4"/>
     </row>
-    <row r="7" spans="2:11" ht="32.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="2:11" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B7" s="8" t="s">
         <v>9</v>
       </c>
@@ -2134,7 +2750,7 @@
       </c>
       <c r="K7" s="4"/>
     </row>
-    <row r="8" spans="2:11" ht="33" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="2:11" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B8" s="8" t="s">
         <v>9</v>
       </c>
@@ -2164,7 +2780,7 @@
       </c>
       <c r="K8" s="4"/>
     </row>
-    <row r="9" spans="2:11" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="2:11" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B9" s="8" t="s">
         <v>9</v>
       </c>
@@ -2194,7 +2810,7 @@
       </c>
       <c r="K9" s="4"/>
     </row>
-    <row r="10" spans="2:11" ht="29" x14ac:dyDescent="0.35">
+    <row r="10" spans="2:11" ht="30" x14ac:dyDescent="0.25">
       <c r="B10" s="8" t="s">
         <v>9</v>
       </c>
@@ -2224,7 +2840,7 @@
       </c>
       <c r="K10" s="4"/>
     </row>
-    <row r="11" spans="2:11" ht="29" x14ac:dyDescent="0.35">
+    <row r="11" spans="2:11" ht="30" x14ac:dyDescent="0.25">
       <c r="B11" s="8" t="s">
         <v>9</v>
       </c>
@@ -2254,7 +2870,7 @@
       </c>
       <c r="K11" s="4"/>
     </row>
-    <row r="12" spans="2:11" ht="29" x14ac:dyDescent="0.35">
+    <row r="12" spans="2:11" ht="30" x14ac:dyDescent="0.25">
       <c r="B12" s="8" t="s">
         <v>9</v>
       </c>
@@ -2284,7 +2900,7 @@
       </c>
       <c r="K12" s="4"/>
     </row>
-    <row r="13" spans="2:11" ht="29" x14ac:dyDescent="0.35">
+    <row r="13" spans="2:11" ht="30" x14ac:dyDescent="0.25">
       <c r="B13" s="8" t="s">
         <v>9</v>
       </c>
@@ -2314,7 +2930,7 @@
       </c>
       <c r="K13" s="4"/>
     </row>
-    <row r="14" spans="2:11" ht="29" x14ac:dyDescent="0.35">
+    <row r="14" spans="2:11" ht="30" x14ac:dyDescent="0.25">
       <c r="B14" s="8" t="s">
         <v>9</v>
       </c>
@@ -2344,7 +2960,7 @@
       </c>
       <c r="K14" s="4"/>
     </row>
-    <row r="15" spans="2:11" ht="29" x14ac:dyDescent="0.35">
+    <row r="15" spans="2:11" ht="30" x14ac:dyDescent="0.25">
       <c r="B15" s="8" t="s">
         <v>9</v>
       </c>
@@ -2374,7 +2990,7 @@
       </c>
       <c r="K15" s="4"/>
     </row>
-    <row r="16" spans="2:11" ht="29" x14ac:dyDescent="0.35">
+    <row r="16" spans="2:11" ht="30" x14ac:dyDescent="0.25">
       <c r="B16" s="8" t="s">
         <v>9</v>
       </c>
@@ -2404,7 +3020,7 @@
       </c>
       <c r="K16" s="4"/>
     </row>
-    <row r="17" spans="2:11" ht="29" x14ac:dyDescent="0.35">
+    <row r="17" spans="2:11" ht="30" x14ac:dyDescent="0.25">
       <c r="B17" s="8" t="s">
         <v>9</v>
       </c>
@@ -2434,7 +3050,7 @@
       </c>
       <c r="K17" s="4"/>
     </row>
-    <row r="18" spans="2:11" ht="29" x14ac:dyDescent="0.35">
+    <row r="18" spans="2:11" ht="30" x14ac:dyDescent="0.25">
       <c r="B18" s="8" t="s">
         <v>9</v>
       </c>
@@ -2464,7 +3080,7 @@
       </c>
       <c r="K18" s="4"/>
     </row>
-    <row r="19" spans="2:11" ht="29" x14ac:dyDescent="0.35">
+    <row r="19" spans="2:11" ht="30" x14ac:dyDescent="0.25">
       <c r="B19" s="8" t="s">
         <v>9</v>
       </c>
@@ -2494,7 +3110,7 @@
       </c>
       <c r="K19" s="4"/>
     </row>
-    <row r="20" spans="2:11" ht="29" x14ac:dyDescent="0.35">
+    <row r="20" spans="2:11" ht="30" x14ac:dyDescent="0.25">
       <c r="B20" s="8" t="s">
         <v>9</v>
       </c>
@@ -2524,7 +3140,7 @@
       </c>
       <c r="K20" s="4"/>
     </row>
-    <row r="21" spans="2:11" ht="29" x14ac:dyDescent="0.35">
+    <row r="21" spans="2:11" ht="30" x14ac:dyDescent="0.25">
       <c r="B21" s="8" t="s">
         <v>9</v>
       </c>
@@ -2554,7 +3170,7 @@
       </c>
       <c r="K21" s="4"/>
     </row>
-    <row r="22" spans="2:11" ht="29" x14ac:dyDescent="0.35">
+    <row r="22" spans="2:11" ht="30" x14ac:dyDescent="0.25">
       <c r="B22" s="8" t="s">
         <v>9</v>
       </c>
@@ -2584,7 +3200,7 @@
       </c>
       <c r="K22" s="4"/>
     </row>
-    <row r="23" spans="2:11" ht="29" x14ac:dyDescent="0.35">
+    <row r="23" spans="2:11" ht="30" x14ac:dyDescent="0.25">
       <c r="B23" s="8" t="s">
         <v>9</v>
       </c>
@@ -2614,7 +3230,7 @@
       </c>
       <c r="K23" s="4"/>
     </row>
-    <row r="24" spans="2:11" x14ac:dyDescent="0.35">
+    <row r="24" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B24" s="8" t="s">
         <v>9</v>
       </c>
@@ -2644,7 +3260,7 @@
       </c>
       <c r="K24" s="4"/>
     </row>
-    <row r="25" spans="2:11" x14ac:dyDescent="0.35">
+    <row r="25" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B25" s="8"/>
       <c r="C25" s="15"/>
       <c r="D25" s="18"/>
@@ -2656,7 +3272,7 @@
       <c r="J25" s="9"/>
       <c r="K25" s="4"/>
     </row>
-    <row r="26" spans="2:11" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="26" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B26" s="8"/>
       <c r="C26" s="15"/>
       <c r="D26" s="18"/>
@@ -2674,63 +3290,895 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:J23"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H30" sqref="H30"/>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <sheetData/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="22.85546875" customWidth="1"/>
+    <col min="2" max="2" width="23.28515625" customWidth="1"/>
+    <col min="3" max="3" width="34.42578125" customWidth="1"/>
+    <col min="4" max="4" width="34" customWidth="1"/>
+    <col min="6" max="6" width="51.140625" customWidth="1"/>
+    <col min="8" max="8" width="15.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" ht="43.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="42" t="s">
+        <v>13</v>
+      </c>
+      <c r="B1" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="C1" s="12" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1" s="12" t="s">
+        <v>1</v>
+      </c>
+      <c r="E1" s="12" t="s">
+        <v>2</v>
+      </c>
+      <c r="F1" s="12" t="s">
+        <v>3</v>
+      </c>
+      <c r="G1" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="H1" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="I1" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="J1" s="14" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="43" t="s">
+        <v>9</v>
+      </c>
+      <c r="B2" s="8" t="s">
+        <v>96</v>
+      </c>
+      <c r="C2" s="9" t="s">
+        <v>54</v>
+      </c>
+      <c r="D2" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="E2" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="F2" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="G2" s="19">
+        <v>44530</v>
+      </c>
+      <c r="H2" s="9" t="s">
+        <v>103</v>
+      </c>
+      <c r="I2" s="9" t="s">
+        <v>39</v>
+      </c>
+      <c r="J2" s="10"/>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A3" s="43" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3" s="8" t="s">
+        <v>97</v>
+      </c>
+      <c r="C3" s="18" t="s">
+        <v>100</v>
+      </c>
+      <c r="D3" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="E3" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="F3" s="9" t="s">
+        <v>104</v>
+      </c>
+      <c r="G3" s="19">
+        <v>44531</v>
+      </c>
+      <c r="H3" s="9" t="s">
+        <v>103</v>
+      </c>
+      <c r="I3" s="9" t="s">
+        <v>39</v>
+      </c>
+      <c r="J3" s="4"/>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A4" s="43" t="s">
+        <v>9</v>
+      </c>
+      <c r="B4" s="8" t="s">
+        <v>98</v>
+      </c>
+      <c r="C4" s="18" t="s">
+        <v>101</v>
+      </c>
+      <c r="D4" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="E4" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="F4" s="9" t="s">
+        <v>105</v>
+      </c>
+      <c r="G4" s="19">
+        <v>44532</v>
+      </c>
+      <c r="H4" s="9" t="s">
+        <v>103</v>
+      </c>
+      <c r="I4" s="9" t="s">
+        <v>39</v>
+      </c>
+      <c r="J4" s="4"/>
+    </row>
+    <row r="5" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="44" t="s">
+        <v>9</v>
+      </c>
+      <c r="B5" s="32" t="s">
+        <v>99</v>
+      </c>
+      <c r="C5" s="34" t="s">
+        <v>102</v>
+      </c>
+      <c r="D5" s="35" t="s">
+        <v>10</v>
+      </c>
+      <c r="E5" s="35" t="s">
+        <v>10</v>
+      </c>
+      <c r="F5" s="35" t="s">
+        <v>106</v>
+      </c>
+      <c r="G5" s="37">
+        <v>44533</v>
+      </c>
+      <c r="H5" s="9" t="s">
+        <v>103</v>
+      </c>
+      <c r="I5" s="35" t="s">
+        <v>39</v>
+      </c>
+      <c r="J5" s="7"/>
+    </row>
+    <row r="6" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="44"/>
+      <c r="B6" s="32"/>
+      <c r="C6" s="34"/>
+      <c r="D6" s="35"/>
+      <c r="E6" s="35"/>
+      <c r="F6" s="45"/>
+      <c r="G6" s="46"/>
+      <c r="H6" s="33"/>
+      <c r="I6" s="35"/>
+      <c r="J6" s="41"/>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A7" s="38"/>
+      <c r="B7" s="38"/>
+      <c r="C7" s="39"/>
+      <c r="D7" s="38"/>
+      <c r="E7" s="38"/>
+      <c r="F7" s="38"/>
+      <c r="G7" s="40"/>
+      <c r="H7" s="38"/>
+      <c r="I7" s="38"/>
+      <c r="J7" s="38"/>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A8" s="38"/>
+      <c r="B8" s="38"/>
+      <c r="C8" s="39"/>
+      <c r="D8" s="38"/>
+      <c r="E8" s="38"/>
+      <c r="F8" s="38"/>
+      <c r="G8" s="40"/>
+      <c r="H8" s="38"/>
+      <c r="I8" s="38"/>
+      <c r="J8" s="38"/>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A9" s="38"/>
+      <c r="B9" s="38"/>
+      <c r="C9" s="39"/>
+      <c r="D9" s="38"/>
+      <c r="E9" s="38"/>
+      <c r="F9" s="39"/>
+      <c r="G9" s="40"/>
+      <c r="H9" s="38"/>
+      <c r="I9" s="38"/>
+      <c r="J9" s="38"/>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A10" s="38"/>
+      <c r="B10" s="38"/>
+      <c r="C10" s="39"/>
+      <c r="D10" s="38"/>
+      <c r="E10" s="38"/>
+      <c r="F10" s="39"/>
+      <c r="G10" s="40"/>
+      <c r="H10" s="38"/>
+      <c r="I10" s="38"/>
+      <c r="J10" s="38"/>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A11" s="38"/>
+      <c r="B11" s="38"/>
+      <c r="C11" s="39"/>
+      <c r="D11" s="38"/>
+      <c r="E11" s="38"/>
+      <c r="F11" s="39"/>
+      <c r="G11" s="40"/>
+      <c r="H11" s="38"/>
+      <c r="I11" s="38"/>
+      <c r="J11" s="38"/>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A12" s="38"/>
+      <c r="B12" s="38"/>
+      <c r="C12" s="39"/>
+      <c r="D12" s="38"/>
+      <c r="E12" s="38"/>
+      <c r="F12" s="39"/>
+      <c r="G12" s="40"/>
+      <c r="H12" s="38"/>
+      <c r="I12" s="38"/>
+      <c r="J12" s="38"/>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A13" s="38"/>
+      <c r="B13" s="38"/>
+      <c r="C13" s="39"/>
+      <c r="D13" s="38"/>
+      <c r="E13" s="38"/>
+      <c r="F13" s="39"/>
+      <c r="G13" s="40"/>
+      <c r="H13" s="38"/>
+      <c r="I13" s="38"/>
+      <c r="J13" s="38"/>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A14" s="38"/>
+      <c r="B14" s="38"/>
+      <c r="C14" s="39"/>
+      <c r="D14" s="38"/>
+      <c r="E14" s="38"/>
+      <c r="F14" s="39"/>
+      <c r="G14" s="40"/>
+      <c r="H14" s="38"/>
+      <c r="I14" s="38"/>
+      <c r="J14" s="38"/>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A15" s="38"/>
+      <c r="B15" s="38"/>
+      <c r="C15" s="39"/>
+      <c r="D15" s="38"/>
+      <c r="E15" s="38"/>
+      <c r="F15" s="39"/>
+      <c r="G15" s="40"/>
+      <c r="H15" s="38"/>
+      <c r="I15" s="38"/>
+      <c r="J15" s="38"/>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A16" s="38"/>
+      <c r="B16" s="38"/>
+      <c r="C16" s="39"/>
+      <c r="D16" s="38"/>
+      <c r="E16" s="38"/>
+      <c r="F16" s="39"/>
+      <c r="G16" s="40"/>
+      <c r="H16" s="38"/>
+      <c r="I16" s="38"/>
+      <c r="J16" s="38"/>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A17" s="38"/>
+      <c r="B17" s="38"/>
+      <c r="C17" s="39"/>
+      <c r="D17" s="38"/>
+      <c r="E17" s="38"/>
+      <c r="F17" s="39"/>
+      <c r="G17" s="40"/>
+      <c r="H17" s="38"/>
+      <c r="I17" s="38"/>
+      <c r="J17" s="38"/>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A18" s="38"/>
+      <c r="B18" s="38"/>
+      <c r="C18" s="39"/>
+      <c r="D18" s="38"/>
+      <c r="E18" s="38"/>
+      <c r="F18" s="39"/>
+      <c r="G18" s="40"/>
+      <c r="H18" s="38"/>
+      <c r="I18" s="38"/>
+      <c r="J18" s="38"/>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A19" s="38"/>
+      <c r="B19" s="38"/>
+      <c r="C19" s="39"/>
+      <c r="D19" s="38"/>
+      <c r="E19" s="38"/>
+      <c r="F19" s="39"/>
+      <c r="G19" s="40"/>
+      <c r="H19" s="38"/>
+      <c r="I19" s="38"/>
+      <c r="J19" s="38"/>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A20" s="38"/>
+      <c r="B20" s="38"/>
+      <c r="C20" s="39"/>
+      <c r="D20" s="38"/>
+      <c r="E20" s="38"/>
+      <c r="F20" s="39"/>
+      <c r="G20" s="40"/>
+      <c r="H20" s="38"/>
+      <c r="I20" s="38"/>
+      <c r="J20" s="38"/>
+    </row>
+    <row r="21" spans="1:10" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="38"/>
+      <c r="B21" s="38"/>
+      <c r="C21" s="39"/>
+      <c r="D21" s="38"/>
+      <c r="E21" s="38"/>
+      <c r="F21" s="38"/>
+      <c r="G21" s="40"/>
+      <c r="H21" s="38"/>
+      <c r="I21" s="38"/>
+      <c r="J21" s="38"/>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A22" s="38"/>
+      <c r="B22" s="38"/>
+      <c r="C22" s="39"/>
+      <c r="D22" s="38"/>
+      <c r="E22" s="38"/>
+      <c r="F22" s="39"/>
+      <c r="G22" s="40"/>
+      <c r="H22" s="38"/>
+      <c r="I22" s="38"/>
+      <c r="J22" s="38"/>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A23" s="38"/>
+      <c r="B23" s="38"/>
+      <c r="C23" s="39"/>
+      <c r="D23" s="38"/>
+      <c r="E23" s="38"/>
+      <c r="F23" s="39"/>
+      <c r="G23" s="40"/>
+      <c r="H23" s="38"/>
+      <c r="I23" s="38"/>
+      <c r="J23" s="38"/>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:J6"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J6" sqref="J6"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <sheetData/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="22" customWidth="1"/>
+    <col min="2" max="2" width="24.85546875" customWidth="1"/>
+    <col min="3" max="3" width="23" customWidth="1"/>
+    <col min="6" max="6" width="41.28515625" customWidth="1"/>
+    <col min="7" max="7" width="11.5703125" customWidth="1"/>
+    <col min="8" max="8" width="12.28515625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" ht="39.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="42" t="s">
+        <v>13</v>
+      </c>
+      <c r="B1" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="C1" s="12" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1" s="12" t="s">
+        <v>1</v>
+      </c>
+      <c r="E1" s="12" t="s">
+        <v>2</v>
+      </c>
+      <c r="F1" s="12" t="s">
+        <v>3</v>
+      </c>
+      <c r="G1" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="H1" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="I1" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="J1" s="14" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A2" s="43" t="s">
+        <v>9</v>
+      </c>
+      <c r="B2" s="8" t="s">
+        <v>107</v>
+      </c>
+      <c r="C2" s="9" t="s">
+        <v>54</v>
+      </c>
+      <c r="D2" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="E2" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="F2" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="G2" s="19">
+        <v>44561</v>
+      </c>
+      <c r="H2" s="9" t="s">
+        <v>103</v>
+      </c>
+      <c r="I2" s="9" t="s">
+        <v>39</v>
+      </c>
+      <c r="J2" s="10"/>
+    </row>
+    <row r="3" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="A3" s="43" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3" s="8" t="s">
+        <v>108</v>
+      </c>
+      <c r="C3" s="18" t="s">
+        <v>111</v>
+      </c>
+      <c r="D3" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="E3" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="F3" s="9" t="s">
+        <v>114</v>
+      </c>
+      <c r="G3" s="19">
+        <v>44562</v>
+      </c>
+      <c r="H3" s="9" t="s">
+        <v>103</v>
+      </c>
+      <c r="I3" s="9" t="s">
+        <v>39</v>
+      </c>
+      <c r="J3" s="4"/>
+    </row>
+    <row r="4" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="A4" s="43" t="s">
+        <v>9</v>
+      </c>
+      <c r="B4" s="8" t="s">
+        <v>109</v>
+      </c>
+      <c r="C4" s="18" t="s">
+        <v>112</v>
+      </c>
+      <c r="D4" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="E4" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="F4" s="9" t="s">
+        <v>115</v>
+      </c>
+      <c r="G4" s="19">
+        <v>44563</v>
+      </c>
+      <c r="H4" s="9" t="s">
+        <v>103</v>
+      </c>
+      <c r="I4" s="9" t="s">
+        <v>39</v>
+      </c>
+      <c r="J4" s="4"/>
+    </row>
+    <row r="5" spans="1:10" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="44" t="s">
+        <v>9</v>
+      </c>
+      <c r="B5" s="8" t="s">
+        <v>110</v>
+      </c>
+      <c r="C5" s="34" t="s">
+        <v>113</v>
+      </c>
+      <c r="D5" s="35" t="s">
+        <v>10</v>
+      </c>
+      <c r="E5" s="35" t="s">
+        <v>10</v>
+      </c>
+      <c r="F5" s="35" t="s">
+        <v>116</v>
+      </c>
+      <c r="G5" s="19">
+        <v>44564</v>
+      </c>
+      <c r="H5" s="9" t="s">
+        <v>103</v>
+      </c>
+      <c r="I5" s="35" t="s">
+        <v>39</v>
+      </c>
+      <c r="J5" s="7"/>
+    </row>
+    <row r="6" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="44"/>
+      <c r="B6" s="32"/>
+      <c r="C6" s="34"/>
+      <c r="D6" s="35"/>
+      <c r="E6" s="35"/>
+      <c r="F6" s="35"/>
+      <c r="G6" s="36"/>
+      <c r="H6" s="35"/>
+      <c r="I6" s="35"/>
+      <c r="J6" s="41"/>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:J4"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <sheetData/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="23" customWidth="1"/>
+    <col min="2" max="2" width="23.42578125" customWidth="1"/>
+    <col min="3" max="3" width="24" customWidth="1"/>
+    <col min="6" max="6" width="43.5703125" customWidth="1"/>
+    <col min="8" max="8" width="16.5703125" customWidth="1"/>
+    <col min="9" max="9" width="15.28515625" customWidth="1"/>
+    <col min="10" max="10" width="15" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" ht="45.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="42" t="s">
+        <v>119</v>
+      </c>
+      <c r="B1" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="C1" s="12" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1" s="12" t="s">
+        <v>1</v>
+      </c>
+      <c r="E1" s="12" t="s">
+        <v>2</v>
+      </c>
+      <c r="F1" s="12" t="s">
+        <v>3</v>
+      </c>
+      <c r="G1" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="H1" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="I1" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="J1" s="14" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A2" s="43" t="s">
+        <v>9</v>
+      </c>
+      <c r="B2" s="8" t="s">
+        <v>117</v>
+      </c>
+      <c r="C2" s="9" t="s">
+        <v>54</v>
+      </c>
+      <c r="D2" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="E2" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="F2" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="G2" s="19">
+        <v>44532</v>
+      </c>
+      <c r="H2" s="9" t="s">
+        <v>103</v>
+      </c>
+      <c r="I2" s="9" t="s">
+        <v>39</v>
+      </c>
+      <c r="J2" s="10"/>
+    </row>
+    <row r="3" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="A3" s="43" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3" s="8" t="s">
+        <v>118</v>
+      </c>
+      <c r="C3" s="18" t="s">
+        <v>120</v>
+      </c>
+      <c r="D3" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="E3" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="F3" s="9" t="s">
+        <v>121</v>
+      </c>
+      <c r="G3" s="19">
+        <v>44533</v>
+      </c>
+      <c r="H3" s="9" t="s">
+        <v>103</v>
+      </c>
+      <c r="I3" s="9" t="s">
+        <v>61</v>
+      </c>
+      <c r="J3" s="4"/>
+    </row>
+    <row r="4" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="A4" s="43" t="s">
+        <v>9</v>
+      </c>
+      <c r="B4" s="8" t="s">
+        <v>118</v>
+      </c>
+      <c r="C4" s="18" t="s">
+        <v>120</v>
+      </c>
+      <c r="D4" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="E4" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="F4" s="9" t="s">
+        <v>122</v>
+      </c>
+      <c r="G4" s="19">
+        <v>44534</v>
+      </c>
+      <c r="H4" s="9" t="s">
+        <v>103</v>
+      </c>
+      <c r="I4" s="9" t="s">
+        <v>39</v>
+      </c>
+      <c r="J4" s="4"/>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:J4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J4" sqref="A1:J4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="23.42578125" customWidth="1"/>
+    <col min="2" max="2" width="22.85546875" customWidth="1"/>
+    <col min="3" max="3" width="32" customWidth="1"/>
+    <col min="4" max="4" width="11" customWidth="1"/>
+    <col min="6" max="6" width="37.85546875" customWidth="1"/>
+    <col min="7" max="7" width="14.5703125" customWidth="1"/>
+    <col min="8" max="8" width="15.5703125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" ht="49.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="42" t="s">
+        <v>119</v>
+      </c>
+      <c r="B1" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="C1" s="12" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1" s="12" t="s">
+        <v>1</v>
+      </c>
+      <c r="E1" s="12" t="s">
+        <v>2</v>
+      </c>
+      <c r="F1" s="12" t="s">
+        <v>3</v>
+      </c>
+      <c r="G1" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="H1" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="I1" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="J1" s="14" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A2" s="43" t="s">
+        <v>9</v>
+      </c>
+      <c r="B2" s="8" t="s">
+        <v>123</v>
+      </c>
+      <c r="C2" s="9" t="s">
+        <v>54</v>
+      </c>
+      <c r="D2" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="E2" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="F2" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="G2" s="19">
+        <v>44532</v>
+      </c>
+      <c r="H2" s="9" t="s">
+        <v>103</v>
+      </c>
+      <c r="I2" s="9" t="s">
+        <v>39</v>
+      </c>
+      <c r="J2" s="10"/>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A3" s="43" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3" s="8" t="s">
+        <v>124</v>
+      </c>
+      <c r="C3" s="18" t="s">
+        <v>125</v>
+      </c>
+      <c r="D3" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="E3" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="F3" s="9" t="s">
+        <v>126</v>
+      </c>
+      <c r="G3" s="19">
+        <v>44533</v>
+      </c>
+      <c r="H3" s="9" t="s">
+        <v>103</v>
+      </c>
+      <c r="I3" s="9" t="s">
+        <v>61</v>
+      </c>
+      <c r="J3" s="4"/>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A4" s="43" t="s">
+        <v>9</v>
+      </c>
+      <c r="B4" s="8" t="s">
+        <v>124</v>
+      </c>
+      <c r="C4" s="18" t="s">
+        <v>125</v>
+      </c>
+      <c r="D4" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="E4" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="F4" s="9" t="s">
+        <v>126</v>
+      </c>
+      <c r="G4" s="19">
+        <v>44534</v>
+      </c>
+      <c r="H4" s="9" t="s">
+        <v>103</v>
+      </c>
+      <c r="I4" s="9" t="s">
+        <v>39</v>
+      </c>
+      <c r="J4" s="4"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J13"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="L13" sqref="L13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="18.7265625" customWidth="1"/>
-    <col min="2" max="2" width="21.7265625" customWidth="1"/>
-    <col min="3" max="3" width="35.54296875" customWidth="1"/>
-    <col min="4" max="4" width="18.1796875" customWidth="1"/>
-    <col min="5" max="5" width="17.453125" customWidth="1"/>
-    <col min="6" max="6" width="33.1796875" customWidth="1"/>
-    <col min="7" max="8" width="14.26953125" customWidth="1"/>
+    <col min="1" max="1" width="18.7109375" customWidth="1"/>
+    <col min="2" max="2" width="21.7109375" customWidth="1"/>
+    <col min="3" max="3" width="35.5703125" customWidth="1"/>
+    <col min="4" max="4" width="18.140625" customWidth="1"/>
+    <col min="5" max="5" width="17.42578125" customWidth="1"/>
+    <col min="6" max="6" width="33.140625" customWidth="1"/>
+    <col min="7" max="8" width="14.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="73" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:10" ht="75.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="11" t="s">
         <v>13</v>
       </c>
@@ -2762,7 +4210,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" s="8" t="s">
         <v>9</v>
       </c>
@@ -2792,7 +4240,7 @@
       </c>
       <c r="J2" s="10"/>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" s="8" t="s">
         <v>9</v>
       </c>
@@ -2822,7 +4270,7 @@
       </c>
       <c r="J3" s="4"/>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" s="8" t="s">
         <v>9</v>
       </c>
@@ -2852,7 +4300,7 @@
       </c>
       <c r="J4" s="4"/>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" s="8" t="s">
         <v>9</v>
       </c>
@@ -2882,7 +4330,7 @@
       </c>
       <c r="J5" s="4"/>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" s="8" t="s">
         <v>9</v>
       </c>
@@ -2912,7 +4360,7 @@
       </c>
       <c r="J6" s="4"/>
     </row>
-    <row r="7" spans="1:10" ht="58" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:10" ht="75" x14ac:dyDescent="0.25">
       <c r="A7" s="20" t="s">
         <v>9</v>
       </c>
@@ -2942,7 +4390,7 @@
       </c>
       <c r="J7" s="4"/>
     </row>
-    <row r="8" spans="1:10" ht="87" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:10" ht="105" x14ac:dyDescent="0.25">
       <c r="A8" s="20" t="s">
         <v>9</v>
       </c>
@@ -2972,7 +4420,7 @@
       </c>
       <c r="J8" s="4"/>
     </row>
-    <row r="9" spans="1:10" ht="58" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:10" ht="60" x14ac:dyDescent="0.25">
       <c r="A9" s="25" t="s">
         <v>9</v>
       </c>
@@ -3001,7 +4449,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="10" spans="1:10" ht="29" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A10" s="25" t="s">
         <v>9</v>
       </c>
@@ -3030,7 +4478,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" s="25" t="s">
         <v>9</v>
       </c>
@@ -3059,7 +4507,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="12" spans="1:10" ht="101.5" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:10" ht="105" x14ac:dyDescent="0.25">
       <c r="A12" s="25" t="s">
         <v>9</v>
       </c>
@@ -3088,7 +4536,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" s="25" t="s">
         <v>9</v>
       </c>

</xml_diff>